<commit_message>
Corrected incorrect other category calculation
</commit_message>
<xml_diff>
--- a/Paper/Results.xlsx
+++ b/Paper/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAE\Semester1\GradWork\git\GradWork\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921704E0-4313-4637-BD70-AFC286EF5896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0378FF-8EEC-40DC-982E-269976CCFD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterSheet" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -493,7 +505,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -591,7 +615,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -689,7 +725,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -787,7 +835,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -869,6 +929,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1277241215"/>
         <c:axId val="1169999872"/>
@@ -1079,6 +1140,56 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mass </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>(800 vs 800)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1091,13 +1202,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1247,6 +1372,62 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'1600vs1600'!$A$3:$A$8</c:f>
@@ -1295,7 +1476,7 @@
                   <c:v>13.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.800000000000011</c:v>
+                  <c:v>7.4000000000000341</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1307,8 +1488,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1415,6 +1597,56 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Multithreading </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>(800 vs 800)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1427,13 +1659,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1583,6 +1829,62 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'1600vs1600'!$A$3:$A$8</c:f>
@@ -1631,7 +1933,7 @@
                   <c:v>17.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.900000000000006</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1643,8 +1945,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1751,6 +2054,56 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Spatial partitioning </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>(800 vs 800)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1763,13 +2116,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1919,6 +2286,62 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'1600vs1600'!$A$3:$A$8</c:f>
@@ -1967,7 +2390,7 @@
                   <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.1</c:v>
+                  <c:v>5.6000000000000014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1979,8 +2402,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2087,6 +2511,56 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Animation sharing </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>(800 vs 800)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2099,13 +2573,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2255,6 +2743,62 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'1600vs1600'!$A$3:$A$8</c:f>
@@ -2303,7 +2847,7 @@
                   <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.399999999999999</c:v>
+                  <c:v>4.1999999999999957</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2315,8 +2859,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2511,7 +3056,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -2609,7 +3166,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -2707,7 +3276,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -2805,7 +3386,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -2903,7 +3496,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -2985,6 +3590,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1378679855"/>
         <c:axId val="1371650383"/>
@@ -3283,7 +3889,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -3381,7 +3999,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -3479,7 +4109,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -3577,7 +4219,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -3675,7 +4329,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -3757,6 +4423,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1379677247"/>
         <c:axId val="265678560"/>
@@ -4054,7 +4721,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -4152,7 +4831,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -4250,7 +4941,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -4348,7 +5051,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -4446,7 +5161,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -4528,6 +5255,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1381939807"/>
         <c:axId val="1371647407"/>
@@ -4826,7 +5554,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -4924,7 +5664,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -5022,7 +5774,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -5120,7 +5884,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -5202,6 +5978,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="271220624"/>
         <c:axId val="265676080"/>
@@ -5501,7 +6278,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -5599,7 +6388,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -5697,7 +6498,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -5795,7 +6608,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -5893,7 +6718,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -5975,6 +6812,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1277892719"/>
         <c:axId val="1504069439"/>
@@ -6269,7 +7107,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -6367,7 +7217,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -6465,7 +7327,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -6563,7 +7437,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -6645,6 +7531,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="271509600"/>
         <c:axId val="1371635007"/>
@@ -6938,7 +7825,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -7036,7 +7935,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -7134,7 +8045,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -7232,7 +8155,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -7330,7 +8265,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -7412,6 +8359,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="260220320"/>
         <c:axId val="265693936"/>
@@ -7622,6 +8570,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Simple (800 vs 800)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7750,6 +8723,62 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:extLst>
@@ -7800,7 +8829,7 @@
                   <c:v>40.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54.600000000000023</c:v>
+                  <c:v>14.400000000000034</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7815,8 +8844,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -15897,10 +16927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -15911,11 +16941,14 @@
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" customWidth="1"/>
     <col min="12" max="12" width="15.77734375" customWidth="1"/>
     <col min="13" max="13" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -15934,344 +16967,341 @@
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="8" cm="1">
-        <f t="array" ref="B2">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B2, "200 vs 200",'200vs200'!B2, "400 vs 400",'400vs400'!B2, "800 vs 800",'800vs800'!B2, "1600 vs 1600",'1600vs1600'!B2, "3200 vs 3200",'3200vs3200'!B2, "6400 vs 6400",'6400vs6400'!B2, "12800 vs 12800",'12800vs12800'!B2)</f>
+        <f t="array" ref="B2">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B2, "200 vs 200",'200vs200'!B2, "400 vs 400",'400vs400'!B2, "800 vs 800",'800vs800'!B2, "1600 vs 1600",'1600vs1600'!B2, "3200 vs 3200",'3200vs3200'!B2, "6400 vs 6400",'6400vs6400'!B2, "12800 vs 12800",'12800vs12800'!B2)</f>
         <v>37.4</v>
       </c>
       <c r="C2" s="8" cm="1">
-        <f t="array" ref="C2">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C2, "200 vs 200",'200vs200'!C2, "400 vs 400",'400vs400'!C2, "800 vs 800",'800vs800'!C2, "1600 vs 1600",'1600vs1600'!C2, "3200 vs 3200",'3200vs3200'!C2, "6400 vs 6400",'6400vs6400'!C2, "12800 vs 12800",'12800vs12800'!C2)</f>
+        <f t="array" ref="C2">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C2, "200 vs 200",'200vs200'!C2, "400 vs 400",'400vs400'!C2, "800 vs 800",'800vs800'!C2, "1600 vs 1600",'1600vs1600'!C2, "3200 vs 3200",'3200vs3200'!C2, "6400 vs 6400",'6400vs6400'!C2, "12800 vs 12800",'12800vs12800'!C2)</f>
         <v>34.4</v>
       </c>
       <c r="D2" s="8" cm="1">
-        <f t="array" ref="D2">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D2, "200 vs 200",'200vs200'!D2, "400 vs 400",'400vs400'!D2, "800 vs 800",'800vs800'!D2, "1600 vs 1600",'1600vs1600'!D2, "3200 vs 3200",'3200vs3200'!D2, "6400 vs 6400",'6400vs6400'!D2, "12800 vs 12800",'12800vs12800'!D2)</f>
+        <f t="array" ref="D2">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D2, "200 vs 200",'200vs200'!D2, "400 vs 400",'400vs400'!D2, "800 vs 800",'800vs800'!D2, "1600 vs 1600",'1600vs1600'!D2, "3200 vs 3200",'3200vs3200'!D2, "6400 vs 6400",'6400vs6400'!D2, "12800 vs 12800",'12800vs12800'!D2)</f>
         <v>19.5</v>
       </c>
       <c r="E2" s="8" cm="1">
-        <f t="array" ref="E2">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E2, "200 vs 200",'200vs200'!E2, "400 vs 400",'400vs400'!E2, "800 vs 800",'800vs800'!E2, "1600 vs 1600",'1600vs1600'!E2, "3200 vs 3200",'3200vs3200'!E2, "6400 vs 6400",'6400vs6400'!E2, "12800 vs 12800",'12800vs12800'!E2)</f>
+        <f t="array" ref="E2">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E2, "200 vs 200",'200vs200'!E2, "400 vs 400",'400vs400'!E2, "800 vs 800",'800vs800'!E2, "1600 vs 1600",'1600vs1600'!E2, "3200 vs 3200",'3200vs3200'!E2, "6400 vs 6400",'6400vs6400'!E2, "12800 vs 12800",'12800vs12800'!E2)</f>
         <v>18.8</v>
       </c>
       <c r="F2" s="8" cm="1">
-        <f t="array" ref="F2">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F2, "200 vs 200",'200vs200'!F2, "400 vs 400",'400vs400'!F2, "800 vs 800",'800vs800'!F2, "1600 vs 1600",'1600vs1600'!F2, "3200 vs 3200",'3200vs3200'!F2, "6400 vs 6400",'6400vs6400'!F2, "12800 vs 12800",'12800vs12800'!F2)</f>
+        <f t="array" ref="F2">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F2, "200 vs 200",'200vs200'!F2, "400 vs 400",'400vs400'!F2, "800 vs 800",'800vs800'!F2, "1600 vs 1600",'1600vs1600'!F2, "3200 vs 3200",'3200vs3200'!F2, "6400 vs 6400",'6400vs6400'!F2, "12800 vs 12800",'12800vs12800'!F2)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="9" cm="1">
-        <f t="array" ref="B3">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B3, "200 vs 200",'200vs200'!B3, "400 vs 400",'400vs400'!B3, "800 vs 800",'800vs800'!B3, "1600 vs 1600",'1600vs1600'!B3, "3200 vs 3200",'3200vs3200'!B3, "6400 vs 6400",'6400vs6400'!B3, "12800 vs 12800",'12800vs12800'!B3)</f>
+        <f t="array" ref="B3">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B3, "200 vs 200",'200vs200'!B3, "400 vs 400",'400vs400'!B3, "800 vs 800",'800vs800'!B3, "1600 vs 1600",'1600vs1600'!B3, "3200 vs 3200",'3200vs3200'!B3, "6400 vs 6400",'6400vs6400'!B3, "12800 vs 12800",'12800vs12800'!B3)</f>
         <v>9.6999999999999993</v>
       </c>
       <c r="C3" s="9" cm="1">
-        <f t="array" ref="C3">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C3, "200 vs 200",'200vs200'!C3, "400 vs 400",'400vs400'!C3, "800 vs 800",'800vs800'!C3, "1600 vs 1600",'1600vs1600'!C3, "3200 vs 3200",'3200vs3200'!C3, "6400 vs 6400",'6400vs6400'!C3, "12800 vs 12800",'12800vs12800'!C3)</f>
+        <f t="array" ref="C3">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C3, "200 vs 200",'200vs200'!C3, "400 vs 400",'400vs400'!C3, "800 vs 800",'800vs800'!C3, "1600 vs 1600",'1600vs1600'!C3, "3200 vs 3200",'3200vs3200'!C3, "6400 vs 6400",'6400vs6400'!C3, "12800 vs 12800",'12800vs12800'!C3)</f>
         <v>11.6</v>
       </c>
       <c r="D3" s="9" cm="1">
-        <f t="array" ref="D3">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D3, "200 vs 200",'200vs200'!D3, "400 vs 400",'400vs400'!D3, "800 vs 800",'800vs800'!D3, "1600 vs 1600",'1600vs1600'!D3, "3200 vs 3200",'3200vs3200'!D3, "6400 vs 6400",'6400vs6400'!D3, "12800 vs 12800",'12800vs12800'!D3)</f>
+        <f t="array" ref="D3">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D3, "200 vs 200",'200vs200'!D3, "400 vs 400",'400vs400'!D3, "800 vs 800",'800vs800'!D3, "1600 vs 1600",'1600vs1600'!D3, "3200 vs 3200",'3200vs3200'!D3, "6400 vs 6400",'6400vs6400'!D3, "12800 vs 12800",'12800vs12800'!D3)</f>
         <v>1.6</v>
       </c>
       <c r="E3" s="9" cm="1">
-        <f t="array" ref="E3">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E3, "200 vs 200",'200vs200'!E3, "400 vs 400",'400vs400'!E3, "800 vs 800",'800vs800'!E3, "1600 vs 1600",'1600vs1600'!E3, "3200 vs 3200",'3200vs3200'!E3, "6400 vs 6400",'6400vs6400'!E3, "12800 vs 12800",'12800vs12800'!E3)</f>
+        <f t="array" ref="E3">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E3, "200 vs 200",'200vs200'!E3, "400 vs 400",'400vs400'!E3, "800 vs 800",'800vs800'!E3, "1600 vs 1600",'1600vs1600'!E3, "3200 vs 3200",'3200vs3200'!E3, "6400 vs 6400",'6400vs6400'!E3, "12800 vs 12800",'12800vs12800'!E3)</f>
         <v>0.9</v>
       </c>
       <c r="F3" s="9" cm="1">
-        <f t="array" ref="F3">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F3, "200 vs 200",'200vs200'!F3, "400 vs 400",'400vs400'!F3, "800 vs 800",'800vs800'!F3, "1600 vs 1600",'1600vs1600'!F3, "3200 vs 3200",'3200vs3200'!F3, "6400 vs 6400",'6400vs6400'!F3, "12800 vs 12800",'12800vs12800'!F3)</f>
+        <f t="array" ref="F3">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F3, "200 vs 200",'200vs200'!F3, "400 vs 400",'400vs400'!F3, "800 vs 800",'800vs800'!F3, "1600 vs 1600",'1600vs1600'!F3, "3200 vs 3200",'3200vs3200'!F3, "6400 vs 6400",'6400vs6400'!F3, "12800 vs 12800",'12800vs12800'!F3)</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="9" t="str" cm="1">
-        <f t="array" ref="B4">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B4, "200 vs 200",'200vs200'!B4, "400 vs 400",'400vs400'!B4, "800 vs 800",'800vs800'!B4, "1600 vs 1600",'1600vs1600'!B4, "3200 vs 3200",'3200vs3200'!B4, "6400 vs 6400",'6400vs6400'!B4, "12800 vs 12800",'12800vs12800'!B4)</f>
+        <f t="array" ref="B4">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B4, "200 vs 200",'200vs200'!B4, "400 vs 400",'400vs400'!B4, "800 vs 800",'800vs800'!B4, "1600 vs 1600",'1600vs1600'!B4, "3200 vs 3200",'3200vs3200'!B4, "6400 vs 6400",'6400vs6400'!B4, "12800 vs 12800",'12800vs12800'!B4)</f>
         <v>/</v>
       </c>
       <c r="C4" s="9" cm="1">
-        <f t="array" ref="C4">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C4, "200 vs 200",'200vs200'!C4, "400 vs 400",'400vs400'!C4, "800 vs 800",'800vs800'!C4, "1600 vs 1600",'1600vs1600'!C4, "3200 vs 3200",'3200vs3200'!C4, "6400 vs 6400",'6400vs6400'!C4, "12800 vs 12800",'12800vs12800'!C4)</f>
+        <f t="array" ref="C4">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C4, "200 vs 200",'200vs200'!C4, "400 vs 400",'400vs400'!C4, "800 vs 800",'800vs800'!C4, "1600 vs 1600",'1600vs1600'!C4, "3200 vs 3200",'3200vs3200'!C4, "6400 vs 6400",'6400vs6400'!C4, "12800 vs 12800",'12800vs12800'!C4)</f>
         <v>7.6</v>
       </c>
       <c r="D4" s="9" cm="1">
-        <f t="array" ref="D4">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D4, "200 vs 200",'200vs200'!D4, "400 vs 400",'400vs400'!D4, "800 vs 800",'800vs800'!D4, "1600 vs 1600",'1600vs1600'!D4, "3200 vs 3200",'3200vs3200'!D4, "6400 vs 6400",'6400vs6400'!D4, "12800 vs 12800",'12800vs12800'!D4)</f>
+        <f t="array" ref="D4">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D4, "200 vs 200",'200vs200'!D4, "400 vs 400",'400vs400'!D4, "800 vs 800",'800vs800'!D4, "1600 vs 1600",'1600vs1600'!D4, "3200 vs 3200",'3200vs3200'!D4, "6400 vs 6400",'6400vs6400'!D4, "12800 vs 12800",'12800vs12800'!D4)</f>
         <v>2.4</v>
       </c>
       <c r="E4" s="9" cm="1">
-        <f t="array" ref="E4">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E4, "200 vs 200",'200vs200'!E4, "400 vs 400",'400vs400'!E4, "800 vs 800",'800vs800'!E4, "1600 vs 1600",'1600vs1600'!E4, "3200 vs 3200",'3200vs3200'!E4, "6400 vs 6400",'6400vs6400'!E4, "12800 vs 12800",'12800vs12800'!E4)</f>
+        <f t="array" ref="E4">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E4, "200 vs 200",'200vs200'!E4, "400 vs 400",'400vs400'!E4, "800 vs 800",'800vs800'!E4, "1600 vs 1600",'1600vs1600'!E4, "3200 vs 3200",'3200vs3200'!E4, "6400 vs 6400",'6400vs6400'!E4, "12800 vs 12800",'12800vs12800'!E4)</f>
         <v>2.7</v>
       </c>
       <c r="F4" s="9" cm="1">
-        <f t="array" ref="F4">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F4, "200 vs 200",'200vs200'!F4, "400 vs 400",'400vs400'!F4, "800 vs 800",'800vs800'!F4, "1600 vs 1600",'1600vs1600'!F4, "3200 vs 3200",'3200vs3200'!F4, "6400 vs 6400",'6400vs6400'!F4, "12800 vs 12800",'12800vs12800'!F4)</f>
+        <f t="array" ref="F4">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F4, "200 vs 200",'200vs200'!F4, "400 vs 400",'400vs400'!F4, "800 vs 800",'800vs800'!F4, "1600 vs 1600",'1600vs1600'!F4, "3200 vs 3200",'3200vs3200'!F4, "6400 vs 6400",'6400vs6400'!F4, "12800 vs 12800",'12800vs12800'!F4)</f>
         <v>2.4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="9" cm="1">
-        <f t="array" ref="B5">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B5, "200 vs 200",'200vs200'!B5, "400 vs 400",'400vs400'!B5, "800 vs 800",'800vs800'!B5, "1600 vs 1600",'1600vs1600'!B5, "3200 vs 3200",'3200vs3200'!B5, "6400 vs 6400",'6400vs6400'!B5, "12800 vs 12800",'12800vs12800'!B5)</f>
+        <f t="array" ref="B5">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B5, "200 vs 200",'200vs200'!B5, "400 vs 400",'400vs400'!B5, "800 vs 800",'800vs800'!B5, "1600 vs 1600",'1600vs1600'!B5, "3200 vs 3200",'3200vs3200'!B5, "6400 vs 6400",'6400vs6400'!B5, "12800 vs 12800",'12800vs12800'!B5)</f>
         <v>13.8</v>
       </c>
       <c r="C5" s="9" cm="1">
-        <f t="array" ref="C5">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C5, "200 vs 200",'200vs200'!C5, "400 vs 400",'400vs400'!C5, "800 vs 800",'800vs800'!C5, "1600 vs 1600",'1600vs1600'!C5, "3200 vs 3200",'3200vs3200'!C5, "6400 vs 6400",'6400vs6400'!C5, "12800 vs 12800",'12800vs12800'!C5)</f>
+        <f t="array" ref="C5">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C5, "200 vs 200",'200vs200'!C5, "400 vs 400",'400vs400'!C5, "800 vs 800",'800vs800'!C5, "1600 vs 1600",'1600vs1600'!C5, "3200 vs 3200",'3200vs3200'!C5, "6400 vs 6400",'6400vs6400'!C5, "12800 vs 12800",'12800vs12800'!C5)</f>
         <v>1.4</v>
       </c>
       <c r="D5" s="9" cm="1">
-        <f t="array" ref="D5">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D5, "200 vs 200",'200vs200'!D5, "400 vs 400",'400vs400'!D5, "800 vs 800",'800vs800'!D5, "1600 vs 1600",'1600vs1600'!D5, "3200 vs 3200",'3200vs3200'!D5, "6400 vs 6400",'6400vs6400'!D5, "12800 vs 12800",'12800vs12800'!D5)</f>
+        <f t="array" ref="D5">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D5, "200 vs 200",'200vs200'!D5, "400 vs 400",'400vs400'!D5, "800 vs 800",'800vs800'!D5, "1600 vs 1600",'1600vs1600'!D5, "3200 vs 3200",'3200vs3200'!D5, "6400 vs 6400",'6400vs6400'!D5, "12800 vs 12800",'12800vs12800'!D5)</f>
         <v>1.5</v>
       </c>
       <c r="E5" s="9" cm="1">
-        <f t="array" ref="E5">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E5, "200 vs 200",'200vs200'!E5, "400 vs 400",'400vs400'!E5, "800 vs 800",'800vs800'!E5, "1600 vs 1600",'1600vs1600'!E5, "3200 vs 3200",'3200vs3200'!E5, "6400 vs 6400",'6400vs6400'!E5, "12800 vs 12800",'12800vs12800'!E5)</f>
+        <f t="array" ref="E5">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E5, "200 vs 200",'200vs200'!E5, "400 vs 400",'400vs400'!E5, "800 vs 800",'800vs800'!E5, "1600 vs 1600",'1600vs1600'!E5, "3200 vs 3200",'3200vs3200'!E5, "6400 vs 6400",'6400vs6400'!E5, "12800 vs 12800",'12800vs12800'!E5)</f>
         <v>1.5</v>
       </c>
       <c r="F5" s="9" cm="1">
-        <f t="array" ref="F5">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F5, "200 vs 200",'200vs200'!F5, "400 vs 400",'400vs400'!F5, "800 vs 800",'800vs800'!F5, "1600 vs 1600",'1600vs1600'!F5, "3200 vs 3200",'3200vs3200'!F5, "6400 vs 6400",'6400vs6400'!F5, "12800 vs 12800",'12800vs12800'!F5)</f>
+        <f t="array" ref="F5">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F5, "200 vs 200",'200vs200'!F5, "400 vs 400",'400vs400'!F5, "800 vs 800",'800vs800'!F5, "1600 vs 1600",'1600vs1600'!F5, "3200 vs 3200",'3200vs3200'!F5, "6400 vs 6400",'6400vs6400'!F5, "12800 vs 12800",'12800vs12800'!F5)</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="9" cm="1">
-        <f t="array" ref="B6">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B6, "200 vs 200",'200vs200'!B6, "400 vs 400",'400vs400'!B6, "800 vs 800",'800vs800'!B6, "1600 vs 1600",'1600vs1600'!B6, "3200 vs 3200",'3200vs3200'!B6, "6400 vs 6400",'6400vs6400'!B6, "12800 vs 12800",'12800vs12800'!B6)</f>
+        <f t="array" ref="B6">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B6, "200 vs 200",'200vs200'!B6, "400 vs 400",'400vs400'!B6, "800 vs 800",'800vs800'!B6, "1600 vs 1600",'1600vs1600'!B6, "3200 vs 3200",'3200vs3200'!B6, "6400 vs 6400",'6400vs6400'!B6, "12800 vs 12800",'12800vs12800'!B6)</f>
         <v>0</v>
       </c>
       <c r="C6" s="9" cm="1">
-        <f t="array" ref="C6">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C6, "200 vs 200",'200vs200'!C6, "400 vs 400",'400vs400'!C6, "800 vs 800",'800vs800'!C6, "1600 vs 1600",'1600vs1600'!C6, "3200 vs 3200",'3200vs3200'!C6, "6400 vs 6400",'6400vs6400'!C6, "12800 vs 12800",'12800vs12800'!C6)</f>
+        <f t="array" ref="C6">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C6, "200 vs 200",'200vs200'!C6, "400 vs 400",'400vs400'!C6, "800 vs 800",'800vs800'!C6, "1600 vs 1600",'1600vs1600'!C6, "3200 vs 3200",'3200vs3200'!C6, "6400 vs 6400",'6400vs6400'!C6, "12800 vs 12800",'12800vs12800'!C6)</f>
         <v>0.96</v>
       </c>
       <c r="D6" s="9" cm="1">
-        <f t="array" ref="D6">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D6, "200 vs 200",'200vs200'!D6, "400 vs 400",'400vs400'!D6, "800 vs 800",'800vs800'!D6, "1600 vs 1600",'1600vs1600'!D6, "3200 vs 3200",'3200vs3200'!D6, "6400 vs 6400",'6400vs6400'!D6, "12800 vs 12800",'12800vs12800'!D6)</f>
+        <f t="array" ref="D6">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D6, "200 vs 200",'200vs200'!D6, "400 vs 400",'400vs400'!D6, "800 vs 800",'800vs800'!D6, "1600 vs 1600",'1600vs1600'!D6, "3200 vs 3200",'3200vs3200'!D6, "6400 vs 6400",'6400vs6400'!D6, "12800 vs 12800",'12800vs12800'!D6)</f>
         <v>1.3</v>
       </c>
       <c r="E6" s="9" cm="1">
-        <f t="array" ref="E6">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E6, "200 vs 200",'200vs200'!E6, "400 vs 400",'400vs400'!E6, "800 vs 800",'800vs800'!E6, "1600 vs 1600",'1600vs1600'!E6, "3200 vs 3200",'3200vs3200'!E6, "6400 vs 6400",'6400vs6400'!E6, "12800 vs 12800",'12800vs12800'!E6)</f>
+        <f t="array" ref="E6">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E6, "200 vs 200",'200vs200'!E6, "400 vs 400",'400vs400'!E6, "800 vs 800",'800vs800'!E6, "1600 vs 1600",'1600vs1600'!E6, "3200 vs 3200",'3200vs3200'!E6, "6400 vs 6400",'6400vs6400'!E6, "12800 vs 12800",'12800vs12800'!E6)</f>
         <v>1.3</v>
       </c>
       <c r="F6" s="9" cm="1">
-        <f t="array" ref="F6">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F6, "200 vs 200",'200vs200'!F6, "400 vs 400",'400vs400'!F6, "800 vs 800",'800vs800'!F6, "1600 vs 1600",'1600vs1600'!F6, "3200 vs 3200",'3200vs3200'!F6, "6400 vs 6400",'6400vs6400'!F6, "12800 vs 12800",'12800vs12800'!F6)</f>
+        <f t="array" ref="F6">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F6, "200 vs 200",'200vs200'!F6, "400 vs 400",'400vs400'!F6, "800 vs 800",'800vs800'!F6, "1600 vs 1600",'1600vs1600'!F6, "3200 vs 3200",'3200vs3200'!F6, "6400 vs 6400",'6400vs6400'!F6, "12800 vs 12800",'12800vs12800'!F6)</f>
         <v>3.1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="10" cm="1">
-        <f t="array" ref="B7">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B7, "200 vs 200",'200vs200'!B7, "400 vs 400",'400vs400'!B7, "800 vs 800",'800vs800'!B7, "1600 vs 1600",'1600vs1600'!B7, "3200 vs 3200",'3200vs3200'!B7, "6400 vs 6400",'6400vs6400'!B7, "12800 vs 12800",'12800vs12800'!B7)</f>
+        <f t="array" ref="B7">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B7, "200 vs 200",'200vs200'!B7, "400 vs 400",'400vs400'!B7, "800 vs 800",'800vs800'!B7, "1600 vs 1600",'1600vs1600'!B7, "3200 vs 3200",'3200vs3200'!B7, "6400 vs 6400",'6400vs6400'!B7, "12800 vs 12800",'12800vs12800'!B7)</f>
         <v>9.6999999999999993</v>
       </c>
       <c r="C7" s="10" cm="1">
-        <f t="array" ref="C7">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C7, "200 vs 200",'200vs200'!C7, "400 vs 400",'400vs400'!C7, "800 vs 800",'800vs800'!C7, "1600 vs 1600",'1600vs1600'!C7, "3200 vs 3200",'3200vs3200'!C7, "6400 vs 6400",'6400vs6400'!C7, "12800 vs 12800",'12800vs12800'!C7)</f>
+        <f t="array" ref="C7">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C7, "200 vs 200",'200vs200'!C7, "400 vs 400",'400vs400'!C7, "800 vs 800",'800vs800'!C7, "1600 vs 1600",'1600vs1600'!C7, "3200 vs 3200",'3200vs3200'!C7, "6400 vs 6400",'6400vs6400'!C7, "12800 vs 12800",'12800vs12800'!C7)</f>
         <v>9.6999999999999993</v>
       </c>
       <c r="D7" s="10" cm="1">
-        <f t="array" ref="D7">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D7, "200 vs 200",'200vs200'!D7, "400 vs 400",'400vs400'!D7, "800 vs 800",'800vs800'!D7, "1600 vs 1600",'1600vs1600'!D7, "3200 vs 3200",'3200vs3200'!D7, "6400 vs 6400",'6400vs6400'!D7, "12800 vs 12800",'12800vs12800'!D7)</f>
+        <f t="array" ref="D7">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D7, "200 vs 200",'200vs200'!D7, "400 vs 400",'400vs400'!D7, "800 vs 800",'800vs800'!D7, "1600 vs 1600",'1600vs1600'!D7, "3200 vs 3200",'3200vs3200'!D7, "6400 vs 6400",'6400vs6400'!D7, "12800 vs 12800",'12800vs12800'!D7)</f>
         <v>9.3000000000000007</v>
       </c>
       <c r="E7" s="10" cm="1">
-        <f t="array" ref="E7">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E7, "200 vs 200",'200vs200'!E7, "400 vs 400",'400vs400'!E7, "800 vs 800",'800vs800'!E7, "1600 vs 1600",'1600vs1600'!E7, "3200 vs 3200",'3200vs3200'!E7, "6400 vs 6400",'6400vs6400'!E7, "12800 vs 12800",'12800vs12800'!E7)</f>
+        <f t="array" ref="E7">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E7, "200 vs 200",'200vs200'!E7, "400 vs 400",'400vs400'!E7, "800 vs 800",'800vs800'!E7, "1600 vs 1600",'1600vs1600'!E7, "3200 vs 3200",'3200vs3200'!E7, "6400 vs 6400",'6400vs6400'!E7, "12800 vs 12800",'12800vs12800'!E7)</f>
         <v>9.6999999999999993</v>
       </c>
       <c r="F7" s="10" cm="1">
-        <f t="array" ref="F7">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F7, "200 vs 200",'200vs200'!F7, "400 vs 400",'400vs400'!F7, "800 vs 800",'800vs800'!F7, "1600 vs 1600",'1600vs1600'!F7, "3200 vs 3200",'3200vs3200'!F7, "6400 vs 6400",'6400vs6400'!F7, "12800 vs 12800",'12800vs12800'!F7)</f>
+        <f t="array" ref="F7">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F7, "200 vs 200",'200vs200'!F7, "400 vs 400",'400vs400'!F7, "800 vs 800",'800vs800'!F7, "1600 vs 1600",'1600vs1600'!F7, "3200 vs 3200",'3200vs3200'!F7, "6400 vs 6400",'6400vs6400'!F7, "12800 vs 12800",'12800vs12800'!F7)</f>
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="9" cm="1">
-        <f t="array" ref="B8">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B8, "200 vs 200",'200vs200'!B8, "400 vs 400",'400vs400'!B8, "800 vs 800",'800vs800'!B8, "1600 vs 1600",'1600vs1600'!B8, "3200 vs 3200",'3200vs3200'!B8, "6400 vs 6400",'6400vs6400'!B8, "12800 vs 12800",'12800vs12800'!B8)</f>
-        <v>13.899999999999999</v>
+        <f t="array" ref="B8">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B8, "200 vs 200",'200vs200'!B8, "400 vs 400",'400vs400'!B8, "800 vs 800",'800vs800'!B8, "1600 vs 1600",'1600vs1600'!B8, "3200 vs 3200",'3200vs3200'!B8, "6400 vs 6400",'6400vs6400'!B8, "12800 vs 12800",'12800vs12800'!B8)</f>
+        <v>4.1999999999999957</v>
       </c>
       <c r="C8" s="9" cm="1">
-        <f t="array" ref="C8">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C8, "200 vs 200",'200vs200'!C8, "400 vs 400",'400vs400'!C8, "800 vs 800",'800vs800'!C8, "1600 vs 1600",'1600vs1600'!C8, "3200 vs 3200",'3200vs3200'!C8, "6400 vs 6400",'6400vs6400'!C8, "12800 vs 12800",'12800vs12800'!C8)</f>
-        <v>12.84</v>
+        <f t="array" ref="C8">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C8, "200 vs 200",'200vs200'!C8, "400 vs 400",'400vs400'!C8, "800 vs 800",'800vs800'!C8, "1600 vs 1600",'1600vs1600'!C8, "3200 vs 3200",'3200vs3200'!C8, "6400 vs 6400",'6400vs6400'!C8, "12800 vs 12800",'12800vs12800'!C8)</f>
+        <v>3.1400000000000006</v>
       </c>
       <c r="D8" s="9" cm="1">
-        <f t="array" ref="D8">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D8, "200 vs 200",'200vs200'!D8, "400 vs 400",'400vs400'!D8, "800 vs 800",'800vs800'!D8, "1600 vs 1600",'1600vs1600'!D8, "3200 vs 3200",'3200vs3200'!D8, "6400 vs 6400",'6400vs6400'!D8, "12800 vs 12800",'12800vs12800'!D8)</f>
-        <v>12.7</v>
+        <f t="array" ref="D8">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D8, "200 vs 200",'200vs200'!D8, "400 vs 400",'400vs400'!D8, "800 vs 800",'800vs800'!D8, "1600 vs 1600",'1600vs1600'!D8, "3200 vs 3200",'3200vs3200'!D8, "6400 vs 6400",'6400vs6400'!D8, "12800 vs 12800",'12800vs12800'!D8)</f>
+        <v>3.3999999999999986</v>
       </c>
       <c r="E8" s="9" cm="1">
-        <f t="array" ref="E8">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E8, "200 vs 200",'200vs200'!E8, "400 vs 400",'400vs400'!E8, "800 vs 800",'800vs800'!E8, "1600 vs 1600",'1600vs1600'!E8, "3200 vs 3200",'3200vs3200'!E8, "6400 vs 6400",'6400vs6400'!E8, "12800 vs 12800",'12800vs12800'!E8)</f>
-        <v>12.400000000000002</v>
+        <f t="array" ref="E8">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E8, "200 vs 200",'200vs200'!E8, "400 vs 400",'400vs400'!E8, "800 vs 800",'800vs800'!E8, "1600 vs 1600",'1600vs1600'!E8, "3200 vs 3200",'3200vs3200'!E8, "6400 vs 6400",'6400vs6400'!E8, "12800 vs 12800",'12800vs12800'!E8)</f>
+        <v>2.7000000000000028</v>
       </c>
       <c r="F8" s="9" cm="1">
-        <f t="array" ref="F8">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F8, "200 vs 200",'200vs200'!F8, "400 vs 400",'400vs400'!F8, "800 vs 800",'800vs800'!F8, "1600 vs 1600",'1600vs1600'!F8, "3200 vs 3200",'3200vs3200'!F8, "6400 vs 6400",'6400vs6400'!F8, "12800 vs 12800",'12800vs12800'!F8)</f>
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+        <f t="array" ref="F8">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F8, "200 vs 200",'200vs200'!F8, "400 vs 400",'400vs400'!F8, "800 vs 800",'800vs800'!F8, "1600 vs 1600",'1600vs1600'!F8, "3200 vs 3200",'3200vs3200'!F8, "6400 vs 6400",'6400vs6400'!F8, "12800 vs 12800",'12800vs12800'!F8)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="10" cm="1">
-        <f t="array" ref="B10">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B10, "200 vs 200",'200vs200'!B10, "400 vs 400",'400vs400'!B10, "800 vs 800",'800vs800'!B10, "1600 vs 1600",'1600vs1600'!B10, "3200 vs 3200",'3200vs3200'!B10, "6400 vs 6400",'6400vs6400'!B10, "12800 vs 12800",'12800vs12800'!B10)</f>
+        <f t="array" ref="B10">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B10, "200 vs 200",'200vs200'!B10, "400 vs 400",'400vs400'!B10, "800 vs 800",'800vs800'!B10, "1600 vs 1600",'1600vs1600'!B10, "3200 vs 3200",'3200vs3200'!B10, "6400 vs 6400",'6400vs6400'!B10, "12800 vs 12800",'12800vs12800'!B10)</f>
         <v>14.5</v>
       </c>
       <c r="C10" s="10" cm="1">
-        <f t="array" ref="C10">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C10, "200 vs 200",'200vs200'!C10, "400 vs 400",'400vs400'!C10, "800 vs 800",'800vs800'!C10, "1600 vs 1600",'1600vs1600'!C10, "3200 vs 3200",'3200vs3200'!C10, "6400 vs 6400",'6400vs6400'!C10, "12800 vs 12800",'12800vs12800'!C10)</f>
+        <f t="array" ref="C10">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C10, "200 vs 200",'200vs200'!C10, "400 vs 400",'400vs400'!C10, "800 vs 800",'800vs800'!C10, "1600 vs 1600",'1600vs1600'!C10, "3200 vs 3200",'3200vs3200'!C10, "6400 vs 6400",'6400vs6400'!C10, "12800 vs 12800",'12800vs12800'!C10)</f>
         <v>13.2</v>
       </c>
       <c r="D10" s="10" cm="1">
-        <f t="array" ref="D10">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D10, "200 vs 200",'200vs200'!D10, "400 vs 400",'400vs400'!D10, "800 vs 800",'800vs800'!D10, "1600 vs 1600",'1600vs1600'!D10, "3200 vs 3200",'3200vs3200'!D10, "6400 vs 6400",'6400vs6400'!D10, "12800 vs 12800",'12800vs12800'!D10)</f>
+        <f t="array" ref="D10">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D10, "200 vs 200",'200vs200'!D10, "400 vs 400",'400vs400'!D10, "800 vs 800",'800vs800'!D10, "1600 vs 1600",'1600vs1600'!D10, "3200 vs 3200",'3200vs3200'!D10, "6400 vs 6400",'6400vs6400'!D10, "12800 vs 12800",'12800vs12800'!D10)</f>
         <v>13.9</v>
       </c>
       <c r="E10" s="10" cm="1">
-        <f t="array" ref="E10">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E10, "200 vs 200",'200vs200'!E10, "400 vs 400",'400vs400'!E10, "800 vs 800",'800vs800'!E10, "1600 vs 1600",'1600vs1600'!E10, "3200 vs 3200",'3200vs3200'!E10, "6400 vs 6400",'6400vs6400'!E10, "12800 vs 12800",'12800vs12800'!E10)</f>
+        <f t="array" ref="E10">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E10, "200 vs 200",'200vs200'!E10, "400 vs 400",'400vs400'!E10, "800 vs 800",'800vs800'!E10, "1600 vs 1600",'1600vs1600'!E10, "3200 vs 3200",'3200vs3200'!E10, "6400 vs 6400",'6400vs6400'!E10, "12800 vs 12800",'12800vs12800'!E10)</f>
         <v>14.3</v>
       </c>
       <c r="F10" s="10" cm="1">
-        <f t="array" ref="F10">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F10, "200 vs 200",'200vs200'!F10, "400 vs 400",'400vs400'!F10, "800 vs 800",'800vs800'!F10, "1600 vs 1600",'1600vs1600'!F10, "3200 vs 3200",'3200vs3200'!F10, "6400 vs 6400",'6400vs6400'!F10, "12800 vs 12800",'12800vs12800'!F10)</f>
+        <f t="array" ref="F10">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F10, "200 vs 200",'200vs200'!F10, "400 vs 400",'400vs400'!F10, "800 vs 800",'800vs800'!F10, "1600 vs 1600",'1600vs1600'!F10, "3200 vs 3200",'3200vs3200'!F10, "6400 vs 6400",'6400vs6400'!F10, "12800 vs 12800",'12800vs12800'!F10)</f>
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="10" cm="1">
-        <f t="array" ref="B12">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B12, "200 vs 200",'200vs200'!B12, "400 vs 400",'400vs400'!B12, "800 vs 800",'800vs800'!B12, "1600 vs 1600",'1600vs1600'!B12, "3200 vs 3200",'3200vs3200'!B12, "6400 vs 6400",'6400vs6400'!B12, "12800 vs 12800",'12800vs12800'!B12)</f>
+        <f t="array" ref="B12">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B12, "200 vs 200",'200vs200'!B12, "400 vs 400",'400vs400'!B12, "800 vs 800",'800vs800'!B12, "1600 vs 1600",'1600vs1600'!B12, "3200 vs 3200",'3200vs3200'!B12, "6400 vs 6400",'6400vs6400'!B12, "12800 vs 12800",'12800vs12800'!B12)</f>
         <v>13</v>
       </c>
       <c r="C12" s="10" cm="1">
-        <f t="array" ref="C12">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C12, "200 vs 200",'200vs200'!C12, "400 vs 400",'400vs400'!C12, "800 vs 800",'800vs800'!C12, "1600 vs 1600",'1600vs1600'!C12, "3200 vs 3200",'3200vs3200'!C12, "6400 vs 6400",'6400vs6400'!C12, "12800 vs 12800",'12800vs12800'!C12)</f>
+        <f t="array" ref="C12">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C12, "200 vs 200",'200vs200'!C12, "400 vs 400",'400vs400'!C12, "800 vs 800",'800vs800'!C12, "1600 vs 1600",'1600vs1600'!C12, "3200 vs 3200",'3200vs3200'!C12, "6400 vs 6400",'6400vs6400'!C12, "12800 vs 12800",'12800vs12800'!C12)</f>
         <v>11.2</v>
       </c>
       <c r="D12" s="10" cm="1">
-        <f t="array" ref="D12">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D12, "200 vs 200",'200vs200'!D12, "400 vs 400",'400vs400'!D12, "800 vs 800",'800vs800'!D12, "1600 vs 1600",'1600vs1600'!D12, "3200 vs 3200",'3200vs3200'!D12, "6400 vs 6400",'6400vs6400'!D12, "12800 vs 12800",'12800vs12800'!D12)</f>
+        <f t="array" ref="D12">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D12, "200 vs 200",'200vs200'!D12, "400 vs 400",'400vs400'!D12, "800 vs 800",'800vs800'!D12, "1600 vs 1600",'1600vs1600'!D12, "3200 vs 3200",'3200vs3200'!D12, "6400 vs 6400",'6400vs6400'!D12, "12800 vs 12800",'12800vs12800'!D12)</f>
         <v>10.8</v>
       </c>
       <c r="E12" s="10" cm="1">
-        <f t="array" ref="E12">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E12, "200 vs 200",'200vs200'!E12, "400 vs 400",'400vs400'!E12, "800 vs 800",'800vs800'!E12, "1600 vs 1600",'1600vs1600'!E12, "3200 vs 3200",'3200vs3200'!E12, "6400 vs 6400",'6400vs6400'!E12, "12800 vs 12800",'12800vs12800'!E12)</f>
+        <f t="array" ref="E12">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E12, "200 vs 200",'200vs200'!E12, "400 vs 400",'400vs400'!E12, "800 vs 800",'800vs800'!E12, "1600 vs 1600",'1600vs1600'!E12, "3200 vs 3200",'3200vs3200'!E12, "6400 vs 6400",'6400vs6400'!E12, "12800 vs 12800",'12800vs12800'!E12)</f>
         <v>10.199999999999999</v>
       </c>
       <c r="F12" s="10" cm="1">
-        <f t="array" ref="F12">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F12, "200 vs 200",'200vs200'!F12, "400 vs 400",'400vs400'!F12, "800 vs 800",'800vs800'!F12, "1600 vs 1600",'1600vs1600'!F12, "3200 vs 3200",'3200vs3200'!F12, "6400 vs 6400",'6400vs6400'!F12, "12800 vs 12800",'12800vs12800'!F12)</f>
+        <f t="array" ref="F12">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F12, "200 vs 200",'200vs200'!F12, "400 vs 400",'400vs400'!F12, "800 vs 800",'800vs800'!F12, "1600 vs 1600",'1600vs1600'!F12, "3200 vs 3200",'3200vs3200'!F12, "6400 vs 6400",'6400vs6400'!F12, "12800 vs 12800",'12800vs12800'!F12)</f>
         <v>8.4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="9" cm="1">
-        <f t="array" ref="B13">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B13, "200 vs 200",'200vs200'!B13, "400 vs 400",'400vs400'!B13, "800 vs 800",'800vs800'!B13, "1600 vs 1600",'1600vs1600'!B13, "3200 vs 3200",'3200vs3200'!B13, "6400 vs 6400",'6400vs6400'!B13, "12800 vs 12800",'12800vs12800'!B13)</f>
+        <f t="array" ref="B13">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B13, "200 vs 200",'200vs200'!B13, "400 vs 400",'400vs400'!B13, "800 vs 800",'800vs800'!B13, "1600 vs 1600",'1600vs1600'!B13, "3200 vs 3200",'3200vs3200'!B13, "6400 vs 6400",'6400vs6400'!B13, "12800 vs 12800",'12800vs12800'!B13)</f>
         <v>1.4</v>
       </c>
       <c r="C13" s="9" cm="1">
-        <f t="array" ref="C13">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C13, "200 vs 200",'200vs200'!C13, "400 vs 400",'400vs400'!C13, "800 vs 800",'800vs800'!C13, "1600 vs 1600",'1600vs1600'!C13, "3200 vs 3200",'3200vs3200'!C13, "6400 vs 6400",'6400vs6400'!C13, "12800 vs 12800",'12800vs12800'!C13)</f>
+        <f t="array" ref="C13">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C13, "200 vs 200",'200vs200'!C13, "400 vs 400",'400vs400'!C13, "800 vs 800",'800vs800'!C13, "1600 vs 1600",'1600vs1600'!C13, "3200 vs 3200",'3200vs3200'!C13, "6400 vs 6400",'6400vs6400'!C13, "12800 vs 12800",'12800vs12800'!C13)</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="D13" s="9" cm="1">
-        <f t="array" ref="D13">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D13, "200 vs 200",'200vs200'!D13, "400 vs 400",'400vs400'!D13, "800 vs 800",'800vs800'!D13, "1600 vs 1600",'1600vs1600'!D13, "3200 vs 3200",'3200vs3200'!D13, "6400 vs 6400",'6400vs6400'!D13, "12800 vs 12800",'12800vs12800'!D13)</f>
+        <f t="array" ref="D13">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D13, "200 vs 200",'200vs200'!D13, "400 vs 400",'400vs400'!D13, "800 vs 800",'800vs800'!D13, "1600 vs 1600",'1600vs1600'!D13, "3200 vs 3200",'3200vs3200'!D13, "6400 vs 6400",'6400vs6400'!D13, "12800 vs 12800",'12800vs12800'!D13)</f>
         <v>2.2999999999999998</v>
       </c>
       <c r="E13" s="9" cm="1">
-        <f t="array" ref="E13">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E13, "200 vs 200",'200vs200'!E13, "400 vs 400",'400vs400'!E13, "800 vs 800",'800vs800'!E13, "1600 vs 1600",'1600vs1600'!E13, "3200 vs 3200",'3200vs3200'!E13, "6400 vs 6400",'6400vs6400'!E13, "12800 vs 12800",'12800vs12800'!E13)</f>
+        <f t="array" ref="E13">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E13, "200 vs 200",'200vs200'!E13, "400 vs 400",'400vs400'!E13, "800 vs 800",'800vs800'!E13, "1600 vs 1600",'1600vs1600'!E13, "3200 vs 3200",'3200vs3200'!E13, "6400 vs 6400",'6400vs6400'!E13, "12800 vs 12800",'12800vs12800'!E13)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="F13" s="9" cm="1">
-        <f t="array" ref="F13">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F13, "200 vs 200",'200vs200'!F13, "400 vs 400",'400vs400'!F13, "800 vs 800",'800vs800'!F13, "1600 vs 1600",'1600vs1600'!F13, "3200 vs 3200",'3200vs3200'!F13, "6400 vs 6400",'6400vs6400'!F13, "12800 vs 12800",'12800vs12800'!F13)</f>
+        <f t="array" ref="F13">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F13, "200 vs 200",'200vs200'!F13, "400 vs 400",'400vs400'!F13, "800 vs 800",'800vs800'!F13, "1600 vs 1600",'1600vs1600'!F13, "3200 vs 3200",'3200vs3200'!F13, "6400 vs 6400",'6400vs6400'!F13, "12800 vs 12800",'12800vs12800'!F13)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="9" cm="1">
-        <f t="array" ref="B14">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B14, "200 vs 200",'200vs200'!B14, "400 vs 400",'400vs400'!B14, "800 vs 800",'800vs800'!B14, "1600 vs 1600",'1600vs1600'!B14, "3200 vs 3200",'3200vs3200'!B14, "6400 vs 6400",'6400vs6400'!B14, "12800 vs 12800",'12800vs12800'!B14)</f>
+        <f t="array" ref="B14">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B14, "200 vs 200",'200vs200'!B14, "400 vs 400",'400vs400'!B14, "800 vs 800",'800vs800'!B14, "1600 vs 1600",'1600vs1600'!B14, "3200 vs 3200",'3200vs3200'!B14, "6400 vs 6400",'6400vs6400'!B14, "12800 vs 12800",'12800vs12800'!B14)</f>
         <v>1.4</v>
       </c>
       <c r="C14" s="9" cm="1">
-        <f t="array" ref="C14">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C14, "200 vs 200",'200vs200'!C14, "400 vs 400",'400vs400'!C14, "800 vs 800",'800vs800'!C14, "1600 vs 1600",'1600vs1600'!C14, "3200 vs 3200",'3200vs3200'!C14, "6400 vs 6400",'6400vs6400'!C14, "12800 vs 12800",'12800vs12800'!C14)</f>
+        <f t="array" ref="C14">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C14, "200 vs 200",'200vs200'!C14, "400 vs 400",'400vs400'!C14, "800 vs 800",'800vs800'!C14, "1600 vs 1600",'1600vs1600'!C14, "3200 vs 3200",'3200vs3200'!C14, "6400 vs 6400",'6400vs6400'!C14, "12800 vs 12800",'12800vs12800'!C14)</f>
         <v>0.8</v>
       </c>
       <c r="D14" s="9" cm="1">
-        <f t="array" ref="D14">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D14, "200 vs 200",'200vs200'!D14, "400 vs 400",'400vs400'!D14, "800 vs 800",'800vs800'!D14, "1600 vs 1600",'1600vs1600'!D14, "3200 vs 3200",'3200vs3200'!D14, "6400 vs 6400",'6400vs6400'!D14, "12800 vs 12800",'12800vs12800'!D14)</f>
+        <f t="array" ref="D14">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D14, "200 vs 200",'200vs200'!D14, "400 vs 400",'400vs400'!D14, "800 vs 800",'800vs800'!D14, "1600 vs 1600",'1600vs1600'!D14, "3200 vs 3200",'3200vs3200'!D14, "6400 vs 6400",'6400vs6400'!D14, "12800 vs 12800",'12800vs12800'!D14)</f>
         <v>0.9</v>
       </c>
       <c r="E14" s="9" cm="1">
-        <f t="array" ref="E14">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E14, "200 vs 200",'200vs200'!E14, "400 vs 400",'400vs400'!E14, "800 vs 800",'800vs800'!E14, "1600 vs 1600",'1600vs1600'!E14, "3200 vs 3200",'3200vs3200'!E14, "6400 vs 6400",'6400vs6400'!E14, "12800 vs 12800",'12800vs12800'!E14)</f>
+        <f t="array" ref="E14">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E14, "200 vs 200",'200vs200'!E14, "400 vs 400",'400vs400'!E14, "800 vs 800",'800vs800'!E14, "1600 vs 1600",'1600vs1600'!E14, "3200 vs 3200",'3200vs3200'!E14, "6400 vs 6400",'6400vs6400'!E14, "12800 vs 12800",'12800vs12800'!E14)</f>
         <v>0.8</v>
       </c>
       <c r="F14" s="9" cm="1">
-        <f t="array" ref="F14">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F14, "200 vs 200",'200vs200'!F14, "400 vs 400",'400vs400'!F14, "800 vs 800",'800vs800'!F14, "1600 vs 1600",'1600vs1600'!F14, "3200 vs 3200",'3200vs3200'!F14, "6400 vs 6400",'6400vs6400'!F14, "12800 vs 12800",'12800vs12800'!F14)</f>
+        <f t="array" ref="F14">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F14, "200 vs 200",'200vs200'!F14, "400 vs 400",'400vs400'!F14, "800 vs 800",'800vs800'!F14, "1600 vs 1600",'1600vs1600'!F14, "3200 vs 3200",'3200vs3200'!F14, "6400 vs 6400",'6400vs6400'!F14, "12800 vs 12800",'12800vs12800'!F14)</f>
         <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="9" cm="1">
-        <f t="array" ref="B15">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B15, "200 vs 200",'200vs200'!B15, "400 vs 400",'400vs400'!B15, "800 vs 800",'800vs800'!B15, "1600 vs 1600",'1600vs1600'!B15, "3200 vs 3200",'3200vs3200'!B15, "6400 vs 6400",'6400vs6400'!B15, "12800 vs 12800",'12800vs12800'!B15)</f>
+        <f t="array" ref="B15">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B15, "200 vs 200",'200vs200'!B15, "400 vs 400",'400vs400'!B15, "800 vs 800",'800vs800'!B15, "1600 vs 1600",'1600vs1600'!B15, "3200 vs 3200",'3200vs3200'!B15, "6400 vs 6400",'6400vs6400'!B15, "12800 vs 12800",'12800vs12800'!B15)</f>
         <v>2.1</v>
       </c>
       <c r="C15" s="9" cm="1">
-        <f t="array" ref="C15">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C15, "200 vs 200",'200vs200'!C15, "400 vs 400",'400vs400'!C15, "800 vs 800",'800vs800'!C15, "1600 vs 1600",'1600vs1600'!C15, "3200 vs 3200",'3200vs3200'!C15, "6400 vs 6400",'6400vs6400'!C15, "12800 vs 12800",'12800vs12800'!C15)</f>
+        <f t="array" ref="C15">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C15, "200 vs 200",'200vs200'!C15, "400 vs 400",'400vs400'!C15, "800 vs 800",'800vs800'!C15, "1600 vs 1600",'1600vs1600'!C15, "3200 vs 3200",'3200vs3200'!C15, "6400 vs 6400",'6400vs6400'!C15, "12800 vs 12800",'12800vs12800'!C15)</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="D15" s="9" cm="1">
-        <f t="array" ref="D15">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D15, "200 vs 200",'200vs200'!D15, "400 vs 400",'400vs400'!D15, "800 vs 800",'800vs800'!D15, "1600 vs 1600",'1600vs1600'!D15, "3200 vs 3200",'3200vs3200'!D15, "6400 vs 6400",'6400vs6400'!D15, "12800 vs 12800",'12800vs12800'!D15)</f>
+        <f t="array" ref="D15">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D15, "200 vs 200",'200vs200'!D15, "400 vs 400",'400vs400'!D15, "800 vs 800",'800vs800'!D15, "1600 vs 1600",'1600vs1600'!D15, "3200 vs 3200",'3200vs3200'!D15, "6400 vs 6400",'6400vs6400'!D15, "12800 vs 12800",'12800vs12800'!D15)</f>
         <v>1.2</v>
       </c>
       <c r="E15" s="9" cm="1">
-        <f t="array" ref="E15">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E15, "200 vs 200",'200vs200'!E15, "400 vs 400",'400vs400'!E15, "800 vs 800",'800vs800'!E15, "1600 vs 1600",'1600vs1600'!E15, "3200 vs 3200",'3200vs3200'!E15, "6400 vs 6400",'6400vs6400'!E15, "12800 vs 12800",'12800vs12800'!E15)</f>
+        <f t="array" ref="E15">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E15, "200 vs 200",'200vs200'!E15, "400 vs 400",'400vs400'!E15, "800 vs 800",'800vs800'!E15, "1600 vs 1600",'1600vs1600'!E15, "3200 vs 3200",'3200vs3200'!E15, "6400 vs 6400",'6400vs6400'!E15, "12800 vs 12800",'12800vs12800'!E15)</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="F15" s="9" cm="1">
-        <f t="array" ref="F15">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F15, "200 vs 200",'200vs200'!F15, "400 vs 400",'400vs400'!F15, "800 vs 800",'800vs800'!F15, "1600 vs 1600",'1600vs1600'!F15, "3200 vs 3200",'3200vs3200'!F15, "6400 vs 6400",'6400vs6400'!F15, "12800 vs 12800",'12800vs12800'!F15)</f>
+        <f t="array" ref="F15">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F15, "200 vs 200",'200vs200'!F15, "400 vs 400",'400vs400'!F15, "800 vs 800",'800vs800'!F15, "1600 vs 1600",'1600vs1600'!F15, "3200 vs 3200",'3200vs3200'!F15, "6400 vs 6400",'6400vs6400'!F15, "12800 vs 12800",'12800vs12800'!F15)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="9" cm="1">
-        <f t="array" ref="B16">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B16, "200 vs 200",'200vs200'!B16, "400 vs 400",'400vs400'!B16, "800 vs 800",'800vs800'!B16, "1600 vs 1600",'1600vs1600'!B16, "3200 vs 3200",'3200vs3200'!B16, "6400 vs 6400",'6400vs6400'!B16, "12800 vs 12800",'12800vs12800'!B16)</f>
+        <f t="array" ref="B16">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B16, "200 vs 200",'200vs200'!B16, "400 vs 400",'400vs400'!B16, "800 vs 800",'800vs800'!B16, "1600 vs 1600",'1600vs1600'!B16, "3200 vs 3200",'3200vs3200'!B16, "6400 vs 6400",'6400vs6400'!B16, "12800 vs 12800",'12800vs12800'!B16)</f>
         <v>2</v>
       </c>
       <c r="C16" s="9" cm="1">
-        <f t="array" ref="C16">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C16, "200 vs 200",'200vs200'!C16, "400 vs 400",'400vs400'!C16, "800 vs 800",'800vs800'!C16, "1600 vs 1600",'1600vs1600'!C16, "3200 vs 3200",'3200vs3200'!C16, "6400 vs 6400",'6400vs6400'!C16, "12800 vs 12800",'12800vs12800'!C16)</f>
+        <f t="array" ref="C16">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C16, "200 vs 200",'200vs200'!C16, "400 vs 400",'400vs400'!C16, "800 vs 800",'800vs800'!C16, "1600 vs 1600",'1600vs1600'!C16, "3200 vs 3200",'3200vs3200'!C16, "6400 vs 6400",'6400vs6400'!C16, "12800 vs 12800",'12800vs12800'!C16)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="D16" s="9" cm="1">
-        <f t="array" ref="D16">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D16, "200 vs 200",'200vs200'!D16, "400 vs 400",'400vs400'!D16, "800 vs 800",'800vs800'!D16, "1600 vs 1600",'1600vs1600'!D16, "3200 vs 3200",'3200vs3200'!D16, "6400 vs 6400",'6400vs6400'!D16, "12800 vs 12800",'12800vs12800'!D16)</f>
+        <f t="array" ref="D16">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D16, "200 vs 200",'200vs200'!D16, "400 vs 400",'400vs400'!D16, "800 vs 800",'800vs800'!D16, "1600 vs 1600",'1600vs1600'!D16, "3200 vs 3200",'3200vs3200'!D16, "6400 vs 6400",'6400vs6400'!D16, "12800 vs 12800",'12800vs12800'!D16)</f>
         <v>1.6</v>
       </c>
       <c r="E16" s="9" cm="1">
-        <f t="array" ref="E16">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E16, "200 vs 200",'200vs200'!E16, "400 vs 400",'400vs400'!E16, "800 vs 800",'800vs800'!E16, "1600 vs 1600",'1600vs1600'!E16, "3200 vs 3200",'3200vs3200'!E16, "6400 vs 6400",'6400vs6400'!E16, "12800 vs 12800",'12800vs12800'!E16)</f>
+        <f t="array" ref="E16">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E16, "200 vs 200",'200vs200'!E16, "400 vs 400",'400vs400'!E16, "800 vs 800",'800vs800'!E16, "1600 vs 1600",'1600vs1600'!E16, "3200 vs 3200",'3200vs3200'!E16, "6400 vs 6400",'6400vs6400'!E16, "12800 vs 12800",'12800vs12800'!E16)</f>
         <v>1.6</v>
       </c>
       <c r="F16" s="9" cm="1">
-        <f t="array" ref="F16">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F16, "200 vs 200",'200vs200'!F16, "400 vs 400",'400vs400'!F16, "800 vs 800",'800vs800'!F16, "1600 vs 1600",'1600vs1600'!F16, "3200 vs 3200",'3200vs3200'!F16, "6400 vs 6400",'6400vs6400'!F16, "12800 vs 12800",'12800vs12800'!F16)</f>
+        <f t="array" ref="F16">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F16, "200 vs 200",'200vs200'!F16, "400 vs 400",'400vs400'!F16, "800 vs 800",'800vs800'!F16, "1600 vs 1600",'1600vs1600'!F16, "3200 vs 3200",'3200vs3200'!F16, "6400 vs 6400",'6400vs6400'!F16, "12800 vs 12800",'12800vs12800'!F16)</f>
         <v>1.6</v>
       </c>
     </row>
@@ -16280,23 +17310,23 @@
         <v>15</v>
       </c>
       <c r="B17" s="10" cm="1">
-        <f t="array" ref="B17">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B17, "200 vs 200",'200vs200'!B17, "400 vs 400",'400vs400'!B17, "800 vs 800",'800vs800'!B17, "1600 vs 1600",'1600vs1600'!B17, "3200 vs 3200",'3200vs3200'!B17, "6400 vs 6400",'6400vs6400'!B17, "12800 vs 12800",'12800vs12800'!B17)</f>
+        <f t="array" ref="B17">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B17, "200 vs 200",'200vs200'!B17, "400 vs 400",'400vs400'!B17, "800 vs 800",'800vs800'!B17, "1600 vs 1600",'1600vs1600'!B17, "3200 vs 3200",'3200vs3200'!B17, "6400 vs 6400",'6400vs6400'!B17, "12800 vs 12800",'12800vs12800'!B17)</f>
         <v>3.3</v>
       </c>
       <c r="C17" s="10" cm="1">
-        <f t="array" ref="C17">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C17, "200 vs 200",'200vs200'!C17, "400 vs 400",'400vs400'!C17, "800 vs 800",'800vs800'!C17, "1600 vs 1600",'1600vs1600'!C17, "3200 vs 3200",'3200vs3200'!C17, "6400 vs 6400",'6400vs6400'!C17, "12800 vs 12800",'12800vs12800'!C17)</f>
+        <f t="array" ref="C17">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C17, "200 vs 200",'200vs200'!C17, "400 vs 400",'400vs400'!C17, "800 vs 800",'800vs800'!C17, "1600 vs 1600",'1600vs1600'!C17, "3200 vs 3200",'3200vs3200'!C17, "6400 vs 6400",'6400vs6400'!C17, "12800 vs 12800",'12800vs12800'!C17)</f>
         <v>3.2</v>
       </c>
       <c r="D17" s="10" cm="1">
-        <f t="array" ref="D17">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D17, "200 vs 200",'200vs200'!D17, "400 vs 400",'400vs400'!D17, "800 vs 800",'800vs800'!D17, "1600 vs 1600",'1600vs1600'!D17, "3200 vs 3200",'3200vs3200'!D17, "6400 vs 6400",'6400vs6400'!D17, "12800 vs 12800",'12800vs12800'!D17)</f>
+        <f t="array" ref="D17">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D17, "200 vs 200",'200vs200'!D17, "400 vs 400",'400vs400'!D17, "800 vs 800",'800vs800'!D17, "1600 vs 1600",'1600vs1600'!D17, "3200 vs 3200",'3200vs3200'!D17, "6400 vs 6400",'6400vs6400'!D17, "12800 vs 12800",'12800vs12800'!D17)</f>
         <v>2.4</v>
       </c>
       <c r="E17" s="10" cm="1">
-        <f t="array" ref="E17">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E17, "200 vs 200",'200vs200'!E17, "400 vs 400",'400vs400'!E17, "800 vs 800",'800vs800'!E17, "1600 vs 1600",'1600vs1600'!E17, "3200 vs 3200",'3200vs3200'!E17, "6400 vs 6400",'6400vs6400'!E17, "12800 vs 12800",'12800vs12800'!E17)</f>
+        <f t="array" ref="E17">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E17, "200 vs 200",'200vs200'!E17, "400 vs 400",'400vs400'!E17, "800 vs 800",'800vs800'!E17, "1600 vs 1600",'1600vs1600'!E17, "3200 vs 3200",'3200vs3200'!E17, "6400 vs 6400",'6400vs6400'!E17, "12800 vs 12800",'12800vs12800'!E17)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="F17" s="10" cm="1">
-        <f t="array" ref="F17">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F17, "200 vs 200",'200vs200'!F17, "400 vs 400",'400vs400'!F17, "800 vs 800",'800vs800'!F17, "1600 vs 1600",'1600vs1600'!F17, "3200 vs 3200",'3200vs3200'!F17, "6400 vs 6400",'6400vs6400'!F17, "12800 vs 12800",'12800vs12800'!F17)</f>
+        <f t="array" ref="F17">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F17, "200 vs 200",'200vs200'!F17, "400 vs 400",'400vs400'!F17, "800 vs 800",'800vs800'!F17, "1600 vs 1600",'1600vs1600'!F17, "3200 vs 3200",'3200vs3200'!F17, "6400 vs 6400",'6400vs6400'!F17, "12800 vs 12800",'12800vs12800'!F17)</f>
         <v>2.1</v>
       </c>
     </row>
@@ -16305,29 +17335,29 @@
         <v>10</v>
       </c>
       <c r="B18" s="9" cm="1">
-        <f t="array" ref="B18">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!B18, "200 vs 200",'200vs200'!B18, "400 vs 400",'400vs400'!B18, "800 vs 800",'800vs800'!B18, "1600 vs 1600",'1600vs1600'!B18, "3200 vs 3200",'3200vs3200'!B18, "6400 vs 6400",'6400vs6400'!B18, "12800 vs 12800",'12800vs12800'!B18)</f>
+        <f t="array" ref="B18">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B18, "200 vs 200",'200vs200'!B18, "400 vs 400",'400vs400'!B18, "800 vs 800",'800vs800'!B18, "1600 vs 1600",'1600vs1600'!B18, "3200 vs 3200",'3200vs3200'!B18, "6400 vs 6400",'6400vs6400'!B18, "12800 vs 12800",'12800vs12800'!B18)</f>
         <v>2.8000000000000007</v>
       </c>
       <c r="C18" s="9" cm="1">
-        <f t="array" ref="C18">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!C18, "200 vs 200",'200vs200'!C18, "400 vs 400",'400vs400'!C18, "800 vs 800",'800vs800'!C18, "1600 vs 1600",'1600vs1600'!C18, "3200 vs 3200",'3200vs3200'!C18, "6400 vs 6400",'6400vs6400'!C18, "12800 vs 12800",'12800vs12800'!C18)</f>
+        <f t="array" ref="C18">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C18, "200 vs 200",'200vs200'!C18, "400 vs 400",'400vs400'!C18, "800 vs 800",'800vs800'!C18, "1600 vs 1600",'1600vs1600'!C18, "3200 vs 3200",'3200vs3200'!C18, "6400 vs 6400",'6400vs6400'!C18, "12800 vs 12800",'12800vs12800'!C18)</f>
         <v>2.7999999999999989</v>
       </c>
       <c r="D18" s="9" cm="1">
-        <f t="array" ref="D18">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!D18, "200 vs 200",'200vs200'!D18, "400 vs 400",'400vs400'!D18, "800 vs 800",'800vs800'!D18, "1600 vs 1600",'1600vs1600'!D18, "3200 vs 3200",'3200vs3200'!D18, "6400 vs 6400",'6400vs6400'!D18, "12800 vs 12800",'12800vs12800'!D18)</f>
+        <f t="array" ref="D18">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D18, "200 vs 200",'200vs200'!D18, "400 vs 400",'400vs400'!D18, "800 vs 800",'800vs800'!D18, "1600 vs 1600",'1600vs1600'!D18, "3200 vs 3200",'3200vs3200'!D18, "6400 vs 6400",'6400vs6400'!D18, "12800 vs 12800",'12800vs12800'!D18)</f>
         <v>2.4000000000000004</v>
       </c>
       <c r="E18" s="9" cm="1">
-        <f t="array" ref="E18">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!E18, "200 vs 200",'200vs200'!E18, "400 vs 400",'400vs400'!E18, "800 vs 800",'800vs800'!E18, "1600 vs 1600",'1600vs1600'!E18, "3200 vs 3200",'3200vs3200'!E18, "6400 vs 6400",'6400vs6400'!E18, "12800 vs 12800",'12800vs12800'!E18)</f>
+        <f t="array" ref="E18">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E18, "200 vs 200",'200vs200'!E18, "400 vs 400",'400vs400'!E18, "800 vs 800",'800vs800'!E18, "1600 vs 1600",'1600vs1600'!E18, "3200 vs 3200",'3200vs3200'!E18, "6400 vs 6400",'6400vs6400'!E18, "12800 vs 12800",'12800vs12800'!E18)</f>
         <v>2.2999999999999998</v>
       </c>
       <c r="F18" s="9" cm="1">
-        <f t="array" ref="F18">_xlfn.SWITCH($M$1, "100 vs 100",'100vs100'!F18, "200 vs 200",'200vs200'!F18, "400 vs 400",'400vs400'!F18, "800 vs 800",'800vs800'!F18, "1600 vs 1600",'1600vs1600'!F18, "3200 vs 3200",'3200vs3200'!F18, "6400 vs 6400",'6400vs6400'!F18, "12800 vs 12800",'12800vs12800'!F18)</f>
+        <f t="array" ref="F18">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F18, "200 vs 200",'200vs200'!F18, "400 vs 400",'400vs400'!F18, "800 vs 800",'800vs800'!F18, "1600 vs 1600",'1600vs1600'!F18, "3200 vs 3200",'3200vs3200'!F18, "6400 vs 6400",'6400vs6400'!F18, "12800 vs 12800",'12800vs12800'!F18)</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1" xr:uid="{DE998A2A-6A50-4801-91CC-73A53EB8F813}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1" xr:uid="{DE998A2A-6A50-4801-91CC-73A53EB8F813}">
       <formula1>"100 vs 100,200 vs 200,400 vs 400,800 vs 800,1600 vs 1600,3200 vs 3200,6400 vs 6400,12800 vs 12800"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16340,8 +17370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4529D9-CDB9-404C-BC65-6587A805F484}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16506,24 +17536,24 @@
         <v>10</v>
       </c>
       <c r="B8" s="15">
-        <f>B2-SUM(B3:B6)</f>
-        <v>700</v>
+        <f>B2-SUM(B3:B7)</f>
+        <v>371</v>
       </c>
       <c r="C8" s="15">
-        <f>C2-SUM(C3:C6)</f>
-        <v>26</v>
+        <f t="shared" ref="C8:F8" si="0">C2-SUM(C3:C7)</f>
+        <v>13</v>
       </c>
       <c r="D8" s="15">
-        <f>D2-SUM(D3:D6)</f>
-        <v>42.500000000000455</v>
+        <f t="shared" si="0"/>
+        <v>28.500000000000455</v>
       </c>
       <c r="E8" s="15">
-        <f>E2-SUM(E3:E6)</f>
-        <v>34.200000000000017</v>
+        <f t="shared" si="0"/>
+        <v>27.400000000000006</v>
       </c>
       <c r="F8" s="15">
-        <f>F2-SUM(F3:F6)</f>
-        <v>13.300000000000011</v>
+        <f t="shared" si="0"/>
+        <v>12.100000000000023</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -16689,19 +17719,19 @@
         <v>33.899999999999977</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" ref="C18:F18" si="0">C12-SUM(C13:C17)</f>
+        <f t="shared" ref="C18:F18" si="1">C12-SUM(C13:C17)</f>
         <v>2.5000000000000284</v>
       </c>
       <c r="D18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3999999999999773</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5999999999999943</v>
       </c>
       <c r="F18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.7999999999999829</v>
       </c>
     </row>
@@ -16720,8 +17750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8C534B-81D2-4FA5-A900-ACABFFE2C9A3}">
   <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V61" sqref="V61"/>
+    <sheetView topLeftCell="A149" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18505,7 +19535,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18668,24 +19698,24 @@
         <v>10</v>
       </c>
       <c r="B8" s="15">
-        <f>B2-SUM(B3:B6)</f>
-        <v>5.8000000000000007</v>
+        <f>B2-SUM(B3:B7)</f>
+        <v>1.8000000000000007</v>
       </c>
       <c r="C8" s="15">
-        <f>C2-SUM(C3:C6)</f>
-        <v>5.2899999999999991</v>
+        <f t="shared" ref="C8:F8" si="0">C2-SUM(C3:C7)</f>
+        <v>1.7899999999999991</v>
       </c>
       <c r="D8" s="15">
-        <f>D2-SUM(D3:D6)</f>
-        <v>4.37</v>
+        <f t="shared" si="0"/>
+        <v>1.5700000000000003</v>
       </c>
       <c r="E8" s="15">
-        <f>E2-SUM(E3:E6)</f>
-        <v>4.7799999999999994</v>
+        <f t="shared" si="0"/>
+        <v>2.0799999999999992</v>
       </c>
       <c r="F8" s="15">
-        <f>F2-SUM(F3:F6)</f>
-        <v>4.1399999999999997</v>
+        <f t="shared" si="0"/>
+        <v>2.1399999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -18851,19 +19881,19 @@
         <v>1.9300000000000006</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" ref="C18:F18" si="0">C12-SUM(C13:C17)</f>
+        <f t="shared" ref="C18:F18" si="1">C12-SUM(C13:C17)</f>
         <v>2</v>
       </c>
       <c r="D18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1899999999999995</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0999999999999996</v>
       </c>
       <c r="F18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3499999999999996</v>
       </c>
     </row>
@@ -18883,7 +19913,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -19046,24 +20076,24 @@
         <v>10</v>
       </c>
       <c r="B8" s="15">
-        <f>B2-SUM(B3:B6)</f>
-        <v>7.8000000000000007</v>
+        <f>B2-SUM(B3:B7)</f>
+        <v>2.8000000000000007</v>
       </c>
       <c r="C8" s="15">
-        <f>C2-SUM(C3:C6)</f>
-        <v>7.8</v>
+        <f t="shared" ref="C8:F8" si="0">C2-SUM(C3:C7)</f>
+        <v>1.7999999999999989</v>
       </c>
       <c r="D8" s="15">
-        <f>D2-SUM(D3:D6)</f>
-        <v>8.23</v>
+        <f t="shared" si="0"/>
+        <v>1.7300000000000004</v>
       </c>
       <c r="E8" s="15">
-        <f>E2-SUM(E3:E6)</f>
-        <v>9.91</v>
+        <f t="shared" si="0"/>
+        <v>2.8099999999999987</v>
       </c>
       <c r="F8" s="15">
-        <f>F2-SUM(F3:F6)</f>
-        <v>4.4800000000000004</v>
+        <f t="shared" si="0"/>
+        <v>1.7800000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -19229,19 +20259,19 @@
         <v>1.9000000000000004</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" ref="C18:F18" si="0">C12-SUM(C13:C17)</f>
+        <f t="shared" ref="C18:F18" si="1">C12-SUM(C13:C17)</f>
         <v>2.1999999999999993</v>
       </c>
       <c r="D18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.4499999999999993</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.0999999999999988</v>
       </c>
       <c r="F18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -19261,7 +20291,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -19424,24 +20454,24 @@
         <v>10</v>
       </c>
       <c r="B8" s="15">
-        <f>B2-SUM(B3:B6)</f>
-        <v>13.899999999999999</v>
+        <f>B2-SUM(B3:B7)</f>
+        <v>4.1999999999999957</v>
       </c>
       <c r="C8" s="15">
-        <f>C2-SUM(C3:C6)</f>
-        <v>12.84</v>
+        <f t="shared" ref="C8:F8" si="0">C2-SUM(C3:C7)</f>
+        <v>3.1400000000000006</v>
       </c>
       <c r="D8" s="15">
-        <f>D2-SUM(D3:D6)</f>
-        <v>12.7</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999999999986</v>
       </c>
       <c r="E8" s="15">
-        <f>E2-SUM(E3:E6)</f>
-        <v>12.400000000000002</v>
+        <f t="shared" si="0"/>
+        <v>2.7000000000000028</v>
       </c>
       <c r="F8" s="15">
-        <f>F2-SUM(F3:F6)</f>
-        <v>8.1</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -19607,19 +20637,19 @@
         <v>2.8000000000000007</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" ref="C18:F18" si="0">C12-SUM(C13:C17)</f>
+        <f t="shared" ref="C18:F18" si="1">C12-SUM(C13:C17)</f>
         <v>2.7999999999999989</v>
       </c>
       <c r="D18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="F18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -19639,7 +20669,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -19803,24 +20833,24 @@
         <v>10</v>
       </c>
       <c r="B8" s="15">
-        <f>B2-SUM(B3:B6)</f>
-        <v>32</v>
+        <f>B2-SUM(B3:B7)</f>
+        <v>11</v>
       </c>
       <c r="C8" s="15">
-        <f>C2-SUM(C3:C6)</f>
-        <v>14.100000000000009</v>
+        <f t="shared" ref="C8:F8" si="0">C2-SUM(C3:C7)</f>
+        <v>4.3000000000000114</v>
       </c>
       <c r="D8" s="15">
-        <f>D2-SUM(D3:D6)</f>
-        <v>15.230000000000002</v>
+        <f t="shared" si="0"/>
+        <v>3.8300000000000018</v>
       </c>
       <c r="E8" s="15">
-        <f>E2-SUM(E3:E6)</f>
-        <v>13.760000000000002</v>
+        <f t="shared" si="0"/>
+        <v>3.2600000000000016</v>
       </c>
       <c r="F8" s="15">
-        <f>F2-SUM(F3:F6)</f>
-        <v>7.0999999999999961</v>
+        <f t="shared" si="0"/>
+        <v>2.7999999999999972</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -19986,19 +21016,19 @@
         <v>6.3999999999999986</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" ref="C18:F18" si="0">C12-SUM(C13:C17)</f>
+        <f t="shared" ref="C18:F18" si="1">C12-SUM(C13:C17)</f>
         <v>5</v>
       </c>
       <c r="D18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1999999999999993</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0999999999999996</v>
       </c>
       <c r="F18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
@@ -20018,7 +21048,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20182,24 +21212,24 @@
         <v>10</v>
       </c>
       <c r="B8" s="15">
-        <f>B2-SUM(B3:B6)</f>
-        <v>54.600000000000023</v>
+        <f>B2-SUM(B3:B7)</f>
+        <v>14.400000000000034</v>
       </c>
       <c r="C8" s="15">
-        <f>C2-SUM(C3:C6)</f>
-        <v>20.800000000000011</v>
+        <f t="shared" ref="C8:F8" si="0">C2-SUM(C3:C7)</f>
+        <v>7.4000000000000341</v>
       </c>
       <c r="D8" s="15">
-        <f>D2-SUM(D3:D6)</f>
-        <v>25.900000000000006</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="E8" s="15">
-        <f>E2-SUM(E3:E6)</f>
-        <v>24.1</v>
+        <f t="shared" si="0"/>
+        <v>5.6000000000000014</v>
       </c>
       <c r="F8" s="15">
-        <f>F2-SUM(F3:F6)</f>
-        <v>10.399999999999999</v>
+        <f t="shared" si="0"/>
+        <v>4.1999999999999957</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -20365,19 +21395,19 @@
         <v>14.599999999999994</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" ref="C18:F18" si="0">C12-SUM(C13:C17)</f>
+        <f t="shared" ref="C18:F18" si="1">C12-SUM(C13:C17)</f>
         <v>7.2999999999999972</v>
       </c>
       <c r="D18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8000000000000007</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3999999999999986</v>
       </c>
       <c r="F18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.3999999999999986</v>
       </c>
     </row>
@@ -20397,7 +21427,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F18"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20562,24 +21592,24 @@
         <v>10</v>
       </c>
       <c r="B8" s="15">
-        <f>B2-SUM(B3:B6)</f>
-        <v>119.79999999999995</v>
+        <f>B2-SUM(B3:B7)</f>
+        <v>42.099999999999909</v>
       </c>
       <c r="C8" s="15">
-        <f>C2-SUM(C3:C6)</f>
-        <v>19.399999999999864</v>
+        <f t="shared" ref="C8:F8" si="0">C2-SUM(C3:C7)</f>
+        <v>6.6999999999998181</v>
       </c>
       <c r="D8" s="15">
-        <f>D2-SUM(D3:D6)</f>
-        <v>24.799999999999983</v>
+        <f t="shared" si="0"/>
+        <v>10.999999999999972</v>
       </c>
       <c r="E8" s="15">
-        <f>E2-SUM(E3:E6)</f>
-        <v>27.1</v>
+        <f t="shared" si="0"/>
+        <v>9.7999999999999972</v>
       </c>
       <c r="F8" s="15">
-        <f>F2-SUM(F3:F6)</f>
-        <v>11.600000000000001</v>
+        <f t="shared" si="0"/>
+        <v>7.1000000000000014</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -20745,19 +21775,19 @@
         <v>8.1000000000000014</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" ref="C18:F18" si="0">C12-SUM(C13:C17)</f>
+        <f t="shared" ref="C18:F18" si="1">C12-SUM(C13:C17)</f>
         <v>8.2000000000000028</v>
       </c>
       <c r="D18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.9000000000000057</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.9999999999999929</v>
       </c>
       <c r="F18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
@@ -20777,7 +21807,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F18"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20941,24 +21971,24 @@
         <v>10</v>
       </c>
       <c r="B8" s="15">
-        <f>B2-SUM(B3:B6)</f>
-        <v>277</v>
+        <f>B2-SUM(B3:B7)</f>
+        <v>110</v>
       </c>
       <c r="C8" s="15">
-        <f>C2-SUM(C3:C6)</f>
-        <v>51.800000000000182</v>
+        <f t="shared" ref="C8:F8" si="0">C2-SUM(C3:C7)</f>
+        <v>36.300000000000182</v>
       </c>
       <c r="D8" s="15">
-        <f>D2-SUM(D3:D6)</f>
-        <v>25.799999999999955</v>
+        <f t="shared" si="0"/>
+        <v>12.899999999999977</v>
       </c>
       <c r="E8" s="15">
-        <f>E2-SUM(E3:E6)</f>
-        <v>29.799999999999997</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="F8" s="15">
-        <f>F2-SUM(F3:F6)</f>
-        <v>11.5</v>
+        <f t="shared" si="0"/>
+        <v>8.7000000000000028</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -21124,19 +22154,19 @@
         <v>21.899999999999977</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" ref="C18:F18" si="0">C12-SUM(C13:C17)</f>
+        <f t="shared" ref="C18:F18" si="1">C12-SUM(C13:C17)</f>
         <v>10.299999999999955</v>
       </c>
       <c r="D18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.3999999999999915</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.6999999999999957</v>
       </c>
       <c r="F18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.9000000000000057</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished discussion, conclusion and future work
</commit_message>
<xml_diff>
--- a/Paper/Results.xlsx
+++ b/Paper/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAE\Semester1\GradWork\git\GradWork\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0378FF-8EEC-40DC-982E-269976CCFD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1817BF3-3D3A-4B4B-8CCB-E30346283233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterSheet" sheetId="1" r:id="rId1"/>
@@ -16929,8 +16929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16971,7 +16971,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -16980,23 +16980,23 @@
       </c>
       <c r="B2" s="8" cm="1">
         <f t="array" ref="B2">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B2, "200 vs 200",'200vs200'!B2, "400 vs 400",'400vs400'!B2, "800 vs 800",'800vs800'!B2, "1600 vs 1600",'1600vs1600'!B2, "3200 vs 3200",'3200vs3200'!B2, "6400 vs 6400",'6400vs6400'!B2, "12800 vs 12800",'12800vs12800'!B2)</f>
-        <v>37.4</v>
+        <v>110.8</v>
       </c>
       <c r="C2" s="8" cm="1">
         <f t="array" ref="C2">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C2, "200 vs 200",'200vs200'!C2, "400 vs 400",'400vs400'!C2, "800 vs 800",'800vs800'!C2, "1600 vs 1600",'1600vs1600'!C2, "3200 vs 3200",'3200vs3200'!C2, "6400 vs 6400",'6400vs6400'!C2, "12800 vs 12800",'12800vs12800'!C2)</f>
-        <v>34.4</v>
+        <v>78.7</v>
       </c>
       <c r="D2" s="8" cm="1">
         <f t="array" ref="D2">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D2, "200 vs 200",'200vs200'!D2, "400 vs 400",'400vs400'!D2, "800 vs 800",'800vs800'!D2, "1600 vs 1600",'1600vs1600'!D2, "3200 vs 3200",'3200vs3200'!D2, "6400 vs 6400",'6400vs6400'!D2, "12800 vs 12800",'12800vs12800'!D2)</f>
-        <v>19.5</v>
+        <v>29.6</v>
       </c>
       <c r="E2" s="8" cm="1">
         <f t="array" ref="E2">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E2, "200 vs 200",'200vs200'!E2, "400 vs 400",'400vs400'!E2, "800 vs 800",'800vs800'!E2, "1600 vs 1600",'1600vs1600'!E2, "3200 vs 3200",'3200vs3200'!E2, "6400 vs 6400",'6400vs6400'!E2, "12800 vs 12800",'12800vs12800'!E2)</f>
-        <v>18.8</v>
+        <v>25.1</v>
       </c>
       <c r="F2" s="8" cm="1">
         <f t="array" ref="F2">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F2, "200 vs 200",'200vs200'!F2, "400 vs 400",'400vs400'!F2, "800 vs 800",'800vs800'!F2, "1600 vs 1600",'1600vs1600'!F2, "3200 vs 3200",'3200vs3200'!F2, "6400 vs 6400",'6400vs6400'!F2, "12800 vs 12800",'12800vs12800'!F2)</f>
-        <v>16</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17005,23 +17005,23 @@
       </c>
       <c r="B3" s="9" cm="1">
         <f t="array" ref="B3">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B3, "200 vs 200",'200vs200'!B3, "400 vs 400",'400vs400'!B3, "800 vs 800",'800vs800'!B3, "1600 vs 1600",'1600vs1600'!B3, "3200 vs 3200",'3200vs3200'!B3, "6400 vs 6400",'6400vs6400'!B3, "12800 vs 12800",'12800vs12800'!B3)</f>
-        <v>9.6999999999999993</v>
+        <v>26.7</v>
       </c>
       <c r="C3" s="9" cm="1">
         <f t="array" ref="C3">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C3, "200 vs 200",'200vs200'!C3, "400 vs 400",'400vs400'!C3, "800 vs 800",'800vs800'!C3, "1600 vs 1600",'1600vs1600'!C3, "3200 vs 3200",'3200vs3200'!C3, "6400 vs 6400",'6400vs6400'!C3, "12800 vs 12800",'12800vs12800'!C3)</f>
-        <v>11.6</v>
+        <v>45</v>
       </c>
       <c r="D3" s="9" cm="1">
         <f t="array" ref="D3">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D3, "200 vs 200",'200vs200'!D3, "400 vs 400",'400vs400'!D3, "800 vs 800",'800vs800'!D3, "1600 vs 1600",'1600vs1600'!D3, "3200 vs 3200",'3200vs3200'!D3, "6400 vs 6400",'6400vs6400'!D3, "12800 vs 12800",'12800vs12800'!D3)</f>
-        <v>1.6</v>
+        <v>5.5</v>
       </c>
       <c r="E3" s="9" cm="1">
         <f t="array" ref="E3">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E3, "200 vs 200",'200vs200'!E3, "400 vs 400",'400vs400'!E3, "800 vs 800",'800vs800'!E3, "1600 vs 1600",'1600vs1600'!E3, "3200 vs 3200",'3200vs3200'!E3, "6400 vs 6400",'6400vs6400'!E3, "12800 vs 12800",'12800vs12800'!E3)</f>
-        <v>0.9</v>
+        <v>1.9</v>
       </c>
       <c r="F3" s="9" cm="1">
         <f t="array" ref="F3">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F3, "200 vs 200",'200vs200'!F3, "400 vs 400",'400vs400'!F3, "800 vs 800",'800vs800'!F3, "1600 vs 1600",'1600vs1600'!F3, "3200 vs 3200",'3200vs3200'!F3, "6400 vs 6400",'6400vs6400'!F3, "12800 vs 12800",'12800vs12800'!F3)</f>
-        <v>0.9</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17034,19 +17034,19 @@
       </c>
       <c r="C4" s="9" cm="1">
         <f t="array" ref="C4">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C4, "200 vs 200",'200vs200'!C4, "400 vs 400",'400vs400'!C4, "800 vs 800",'800vs800'!C4, "1600 vs 1600",'1600vs1600'!C4, "3200 vs 3200",'3200vs3200'!C4, "6400 vs 6400",'6400vs6400'!C4, "12800 vs 12800",'12800vs12800'!C4)</f>
-        <v>7.6</v>
+        <v>16</v>
       </c>
       <c r="D4" s="9" cm="1">
         <f t="array" ref="D4">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D4, "200 vs 200",'200vs200'!D4, "400 vs 400",'400vs400'!D4, "800 vs 800",'800vs800'!D4, "1600 vs 1600",'1600vs1600'!D4, "3200 vs 3200",'3200vs3200'!D4, "6400 vs 6400",'6400vs6400'!D4, "12800 vs 12800",'12800vs12800'!D4)</f>
-        <v>2.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E4" s="9" cm="1">
         <f t="array" ref="E4">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E4, "200 vs 200",'200vs200'!E4, "400 vs 400",'400vs400'!E4, "800 vs 800",'800vs800'!E4, "1600 vs 1600",'1600vs1600'!E4, "3200 vs 3200",'3200vs3200'!E4, "6400 vs 6400",'6400vs6400'!E4, "12800 vs 12800",'12800vs12800'!E4)</f>
-        <v>2.7</v>
+        <v>5.2</v>
       </c>
       <c r="F4" s="9" cm="1">
         <f t="array" ref="F4">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F4, "200 vs 200",'200vs200'!F4, "400 vs 400",'400vs400'!F4, "800 vs 800",'800vs800'!F4, "1600 vs 1600",'1600vs1600'!F4, "3200 vs 3200",'3200vs3200'!F4, "6400 vs 6400",'6400vs6400'!F4, "12800 vs 12800",'12800vs12800'!F4)</f>
-        <v>2.4</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17055,23 +17055,23 @@
       </c>
       <c r="B5" s="9" cm="1">
         <f t="array" ref="B5">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B5, "200 vs 200",'200vs200'!B5, "400 vs 400",'400vs400'!B5, "800 vs 800",'800vs800'!B5, "1600 vs 1600",'1600vs1600'!B5, "3200 vs 3200",'3200vs3200'!B5, "6400 vs 6400",'6400vs6400'!B5, "12800 vs 12800",'12800vs12800'!B5)</f>
-        <v>13.8</v>
+        <v>52.1</v>
       </c>
       <c r="C5" s="9" cm="1">
         <f t="array" ref="C5">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C5, "200 vs 200",'200vs200'!C5, "400 vs 400",'400vs400'!C5, "800 vs 800",'800vs800'!C5, "1600 vs 1600",'1600vs1600'!C5, "3200 vs 3200",'3200vs3200'!C5, "6400 vs 6400",'6400vs6400'!C5, "12800 vs 12800",'12800vs12800'!C5)</f>
-        <v>1.4</v>
+        <v>2.8</v>
       </c>
       <c r="D5" s="9" cm="1">
         <f t="array" ref="D5">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D5, "200 vs 200",'200vs200'!D5, "400 vs 400",'400vs400'!D5, "800 vs 800",'800vs800'!D5, "1600 vs 1600",'1600vs1600'!D5, "3200 vs 3200",'3200vs3200'!D5, "6400 vs 6400",'6400vs6400'!D5, "12800 vs 12800",'12800vs12800'!D5)</f>
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="E5" s="9" cm="1">
         <f t="array" ref="E5">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E5, "200 vs 200",'200vs200'!E5, "400 vs 400",'400vs400'!E5, "800 vs 800",'800vs800'!E5, "1600 vs 1600",'1600vs1600'!E5, "3200 vs 3200",'3200vs3200'!E5, "6400 vs 6400",'6400vs6400'!E5, "12800 vs 12800",'12800vs12800'!E5)</f>
-        <v>1.5</v>
+        <v>3.4</v>
       </c>
       <c r="F5" s="9" cm="1">
         <f t="array" ref="F5">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F5, "200 vs 200",'200vs200'!F5, "400 vs 400",'400vs400'!F5, "800 vs 800",'800vs800'!F5, "1600 vs 1600",'1600vs1600'!F5, "3200 vs 3200",'3200vs3200'!F5, "6400 vs 6400",'6400vs6400'!F5, "12800 vs 12800",'12800vs12800'!F5)</f>
-        <v>1.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17084,19 +17084,19 @@
       </c>
       <c r="C6" s="9" cm="1">
         <f t="array" ref="C6">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C6, "200 vs 200",'200vs200'!C6, "400 vs 400",'400vs400'!C6, "800 vs 800",'800vs800'!C6, "1600 vs 1600",'1600vs1600'!C6, "3200 vs 3200",'3200vs3200'!C6, "6400 vs 6400",'6400vs6400'!C6, "12800 vs 12800",'12800vs12800'!C6)</f>
-        <v>0.96</v>
+        <v>0.8</v>
       </c>
       <c r="D6" s="9" cm="1">
         <f t="array" ref="D6">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D6, "200 vs 200",'200vs200'!D6, "400 vs 400",'400vs400'!D6, "800 vs 800",'800vs800'!D6, "1600 vs 1600",'1600vs1600'!D6, "3200 vs 3200",'3200vs3200'!D6, "6400 vs 6400",'6400vs6400'!D6, "12800 vs 12800",'12800vs12800'!D6)</f>
-        <v>1.3</v>
+        <v>0.77</v>
       </c>
       <c r="E6" s="9" cm="1">
         <f t="array" ref="E6">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E6, "200 vs 200",'200vs200'!E6, "400 vs 400",'400vs400'!E6, "800 vs 800",'800vs800'!E6, "1600 vs 1600",'1600vs1600'!E6, "3200 vs 3200",'3200vs3200'!E6, "6400 vs 6400",'6400vs6400'!E6, "12800 vs 12800",'12800vs12800'!E6)</f>
-        <v>1.3</v>
+        <v>0.84</v>
       </c>
       <c r="F6" s="9" cm="1">
         <f t="array" ref="F6">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F6, "200 vs 200",'200vs200'!F6, "400 vs 400",'400vs400'!F6, "800 vs 800",'800vs800'!F6, "1600 vs 1600",'1600vs1600'!F6, "3200 vs 3200",'3200vs3200'!F6, "6400 vs 6400",'6400vs6400'!F6, "12800 vs 12800",'12800vs12800'!F6)</f>
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17105,23 +17105,23 @@
       </c>
       <c r="B7" s="10" cm="1">
         <f t="array" ref="B7">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B7, "200 vs 200",'200vs200'!B7, "400 vs 400",'400vs400'!B7, "800 vs 800",'800vs800'!B7, "1600 vs 1600",'1600vs1600'!B7, "3200 vs 3200",'3200vs3200'!B7, "6400 vs 6400",'6400vs6400'!B7, "12800 vs 12800",'12800vs12800'!B7)</f>
-        <v>9.6999999999999993</v>
+        <v>21</v>
       </c>
       <c r="C7" s="10" cm="1">
         <f t="array" ref="C7">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C7, "200 vs 200",'200vs200'!C7, "400 vs 400",'400vs400'!C7, "800 vs 800",'800vs800'!C7, "1600 vs 1600",'1600vs1600'!C7, "3200 vs 3200",'3200vs3200'!C7, "6400 vs 6400",'6400vs6400'!C7, "12800 vs 12800",'12800vs12800'!C7)</f>
-        <v>9.6999999999999993</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D7" s="10" cm="1">
         <f t="array" ref="D7">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D7, "200 vs 200",'200vs200'!D7, "400 vs 400",'400vs400'!D7, "800 vs 800",'800vs800'!D7, "1600 vs 1600",'1600vs1600'!D7, "3200 vs 3200",'3200vs3200'!D7, "6400 vs 6400",'6400vs6400'!D7, "12800 vs 12800",'12800vs12800'!D7)</f>
-        <v>9.3000000000000007</v>
+        <v>11.4</v>
       </c>
       <c r="E7" s="10" cm="1">
         <f t="array" ref="E7">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E7, "200 vs 200",'200vs200'!E7, "400 vs 400",'400vs400'!E7, "800 vs 800",'800vs800'!E7, "1600 vs 1600",'1600vs1600'!E7, "3200 vs 3200",'3200vs3200'!E7, "6400 vs 6400",'6400vs6400'!E7, "12800 vs 12800",'12800vs12800'!E7)</f>
-        <v>9.6999999999999993</v>
+        <v>10.5</v>
       </c>
       <c r="F7" s="10" cm="1">
         <f t="array" ref="F7">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F7, "200 vs 200",'200vs200'!F7, "400 vs 400",'400vs400'!F7, "800 vs 800",'800vs800'!F7, "1600 vs 1600",'1600vs1600'!F7, "3200 vs 3200",'3200vs3200'!F7, "6400 vs 6400",'6400vs6400'!F7, "12800 vs 12800",'12800vs12800'!F7)</f>
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17130,23 +17130,23 @@
       </c>
       <c r="B8" s="9" cm="1">
         <f t="array" ref="B8">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B8, "200 vs 200",'200vs200'!B8, "400 vs 400",'400vs400'!B8, "800 vs 800",'800vs800'!B8, "1600 vs 1600",'1600vs1600'!B8, "3200 vs 3200",'3200vs3200'!B8, "6400 vs 6400",'6400vs6400'!B8, "12800 vs 12800",'12800vs12800'!B8)</f>
-        <v>4.1999999999999957</v>
+        <v>11</v>
       </c>
       <c r="C8" s="9" cm="1">
         <f t="array" ref="C8">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C8, "200 vs 200",'200vs200'!C8, "400 vs 400",'400vs400'!C8, "800 vs 800",'800vs800'!C8, "1600 vs 1600",'1600vs1600'!C8, "3200 vs 3200",'3200vs3200'!C8, "6400 vs 6400",'6400vs6400'!C8, "12800 vs 12800",'12800vs12800'!C8)</f>
-        <v>3.1400000000000006</v>
+        <v>4.3000000000000114</v>
       </c>
       <c r="D8" s="9" cm="1">
         <f t="array" ref="D8">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D8, "200 vs 200",'200vs200'!D8, "400 vs 400",'400vs400'!D8, "800 vs 800",'800vs800'!D8, "1600 vs 1600",'1600vs1600'!D8, "3200 vs 3200",'3200vs3200'!D8, "6400 vs 6400",'6400vs6400'!D8, "12800 vs 12800",'12800vs12800'!D8)</f>
-        <v>3.3999999999999986</v>
+        <v>3.8300000000000018</v>
       </c>
       <c r="E8" s="9" cm="1">
         <f t="array" ref="E8">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E8, "200 vs 200",'200vs200'!E8, "400 vs 400",'400vs400'!E8, "800 vs 800",'800vs800'!E8, "1600 vs 1600",'1600vs1600'!E8, "3200 vs 3200",'3200vs3200'!E8, "6400 vs 6400",'6400vs6400'!E8, "12800 vs 12800",'12800vs12800'!E8)</f>
-        <v>2.7000000000000028</v>
+        <v>3.2600000000000016</v>
       </c>
       <c r="F8" s="9" cm="1">
         <f t="array" ref="F8">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F8, "200 vs 200",'200vs200'!F8, "400 vs 400",'400vs400'!F8, "800 vs 800",'800vs800'!F8, "1600 vs 1600",'1600vs1600'!F8, "3200 vs 3200",'3200vs3200'!F8, "6400 vs 6400",'6400vs6400'!F8, "12800 vs 12800",'12800vs12800'!F8)</f>
-        <v>4</v>
+        <v>2.7999999999999972</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17158,23 +17158,23 @@
       </c>
       <c r="B10" s="10" cm="1">
         <f t="array" ref="B10">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B10, "200 vs 200",'200vs200'!B10, "400 vs 400",'400vs400'!B10, "800 vs 800",'800vs800'!B10, "1600 vs 1600",'1600vs1600'!B10, "3200 vs 3200",'3200vs3200'!B10, "6400 vs 6400",'6400vs6400'!B10, "12800 vs 12800",'12800vs12800'!B10)</f>
-        <v>14.5</v>
+        <v>28</v>
       </c>
       <c r="C10" s="10" cm="1">
         <f t="array" ref="C10">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C10, "200 vs 200",'200vs200'!C10, "400 vs 400",'400vs400'!C10, "800 vs 800",'800vs800'!C10, "1600 vs 1600",'1600vs1600'!C10, "3200 vs 3200",'3200vs3200'!C10, "6400 vs 6400",'6400vs6400'!C10, "12800 vs 12800",'12800vs12800'!C10)</f>
-        <v>13.2</v>
+        <v>16.2</v>
       </c>
       <c r="D10" s="10" cm="1">
         <f t="array" ref="D10">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D10, "200 vs 200",'200vs200'!D10, "400 vs 400",'400vs400'!D10, "800 vs 800",'800vs800'!D10, "1600 vs 1600",'1600vs1600'!D10, "3200 vs 3200",'3200vs3200'!D10, "6400 vs 6400",'6400vs6400'!D10, "12800 vs 12800",'12800vs12800'!D10)</f>
-        <v>13.9</v>
+        <v>15.7</v>
       </c>
       <c r="E10" s="10" cm="1">
         <f t="array" ref="E10">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E10, "200 vs 200",'200vs200'!E10, "400 vs 400",'400vs400'!E10, "800 vs 800",'800vs800'!E10, "1600 vs 1600",'1600vs1600'!E10, "3200 vs 3200",'3200vs3200'!E10, "6400 vs 6400",'6400vs6400'!E10, "12800 vs 12800",'12800vs12800'!E10)</f>
-        <v>14.3</v>
+        <v>16</v>
       </c>
       <c r="F10" s="10" cm="1">
         <f t="array" ref="F10">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F10, "200 vs 200",'200vs200'!F10, "400 vs 400",'400vs400'!F10, "800 vs 800",'800vs800'!F10, "1600 vs 1600",'1600vs1600'!F10, "3200 vs 3200",'3200vs3200'!F10, "6400 vs 6400",'6400vs6400'!F10, "12800 vs 12800",'12800vs12800'!F10)</f>
-        <v>17.100000000000001</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17186,23 +17186,23 @@
       </c>
       <c r="B12" s="10" cm="1">
         <f t="array" ref="B12">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B12, "200 vs 200",'200vs200'!B12, "400 vs 400",'400vs400'!B12, "800 vs 800",'800vs800'!B12, "1600 vs 1600",'1600vs1600'!B12, "3200 vs 3200",'3200vs3200'!B12, "6400 vs 6400",'6400vs6400'!B12, "12800 vs 12800",'12800vs12800'!B12)</f>
-        <v>13</v>
+        <v>36.4</v>
       </c>
       <c r="C12" s="10" cm="1">
         <f t="array" ref="C12">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C12, "200 vs 200",'200vs200'!C12, "400 vs 400",'400vs400'!C12, "800 vs 800",'800vs800'!C12, "1600 vs 1600",'1600vs1600'!C12, "3200 vs 3200",'3200vs3200'!C12, "6400 vs 6400",'6400vs6400'!C12, "12800 vs 12800",'12800vs12800'!C12)</f>
-        <v>11.2</v>
+        <v>24.5</v>
       </c>
       <c r="D12" s="10" cm="1">
         <f t="array" ref="D12">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D12, "200 vs 200",'200vs200'!D12, "400 vs 400",'400vs400'!D12, "800 vs 800",'800vs800'!D12, "1600 vs 1600",'1600vs1600'!D12, "3200 vs 3200",'3200vs3200'!D12, "6400 vs 6400",'6400vs6400'!D12, "12800 vs 12800",'12800vs12800'!D12)</f>
-        <v>10.8</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="E12" s="10" cm="1">
         <f t="array" ref="E12">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E12, "200 vs 200",'200vs200'!E12, "400 vs 400",'400vs400'!E12, "800 vs 800",'800vs800'!E12, "1600 vs 1600",'1600vs1600'!E12, "3200 vs 3200",'3200vs3200'!E12, "6400 vs 6400",'6400vs6400'!E12, "12800 vs 12800",'12800vs12800'!E12)</f>
-        <v>10.199999999999999</v>
+        <v>8.9</v>
       </c>
       <c r="F12" s="10" cm="1">
         <f t="array" ref="F12">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F12, "200 vs 200",'200vs200'!F12, "400 vs 400",'400vs400'!F12, "800 vs 800",'800vs800'!F12, "1600 vs 1600",'1600vs1600'!F12, "3200 vs 3200",'3200vs3200'!F12, "6400 vs 6400",'6400vs6400'!F12, "12800 vs 12800",'12800vs12800'!F12)</f>
-        <v>8.4</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17211,23 +17211,23 @@
       </c>
       <c r="B13" s="9" cm="1">
         <f t="array" ref="B13">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B13, "200 vs 200",'200vs200'!B13, "400 vs 400",'400vs400'!B13, "800 vs 800",'800vs800'!B13, "1600 vs 1600",'1600vs1600'!B13, "3200 vs 3200",'3200vs3200'!B13, "6400 vs 6400",'6400vs6400'!B13, "12800 vs 12800",'12800vs12800'!B13)</f>
-        <v>1.4</v>
+        <v>4.8</v>
       </c>
       <c r="C13" s="9" cm="1">
         <f t="array" ref="C13">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C13, "200 vs 200",'200vs200'!C13, "400 vs 400",'400vs400'!C13, "800 vs 800",'800vs800'!C13, "1600 vs 1600",'1600vs1600'!C13, "3200 vs 3200",'3200vs3200'!C13, "6400 vs 6400",'6400vs6400'!C13, "12800 vs 12800",'12800vs12800'!C13)</f>
-        <v>1.1000000000000001</v>
+        <v>2.8</v>
       </c>
       <c r="D13" s="9" cm="1">
         <f t="array" ref="D13">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D13, "200 vs 200",'200vs200'!D13, "400 vs 400",'400vs400'!D13, "800 vs 800",'800vs800'!D13, "1600 vs 1600",'1600vs1600'!D13, "3200 vs 3200",'3200vs3200'!D13, "6400 vs 6400",'6400vs6400'!D13, "12800 vs 12800",'12800vs12800'!D13)</f>
-        <v>2.2999999999999998</v>
+        <v>0.9</v>
       </c>
       <c r="E13" s="9" cm="1">
         <f t="array" ref="E13">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E13, "200 vs 200",'200vs200'!E13, "400 vs 400",'400vs400'!E13, "800 vs 800",'800vs800'!E13, "1600 vs 1600",'1600vs1600'!E13, "3200 vs 3200",'3200vs3200'!E13, "6400 vs 6400",'6400vs6400'!E13, "12800 vs 12800",'12800vs12800'!E13)</f>
-        <v>2.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="F13" s="9" cm="1">
         <f t="array" ref="F13">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F13, "200 vs 200",'200vs200'!F13, "400 vs 400",'400vs400'!F13, "800 vs 800",'800vs800'!F13, "1600 vs 1600",'1600vs1600'!F13, "3200 vs 3200",'3200vs3200'!F13, "6400 vs 6400",'6400vs6400'!F13, "12800 vs 12800",'12800vs12800'!F13)</f>
-        <v>1</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17236,11 +17236,11 @@
       </c>
       <c r="B14" s="9" cm="1">
         <f t="array" ref="B14">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B14, "200 vs 200",'200vs200'!B14, "400 vs 400",'400vs400'!B14, "800 vs 800",'800vs800'!B14, "1600 vs 1600",'1600vs1600'!B14, "3200 vs 3200",'3200vs3200'!B14, "6400 vs 6400",'6400vs6400'!B14, "12800 vs 12800",'12800vs12800'!B14)</f>
-        <v>1.4</v>
+        <v>4.5</v>
       </c>
       <c r="C14" s="9" cm="1">
         <f t="array" ref="C14">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C14, "200 vs 200",'200vs200'!C14, "400 vs 400",'400vs400'!C14, "800 vs 800",'800vs800'!C14, "1600 vs 1600",'1600vs1600'!C14, "3200 vs 3200",'3200vs3200'!C14, "6400 vs 6400",'6400vs6400'!C14, "12800 vs 12800",'12800vs12800'!C14)</f>
-        <v>0.8</v>
+        <v>1.7</v>
       </c>
       <c r="D14" s="9" cm="1">
         <f t="array" ref="D14">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D14, "200 vs 200",'200vs200'!D14, "400 vs 400",'400vs400'!D14, "800 vs 800",'800vs800'!D14, "1600 vs 1600",'1600vs1600'!D14, "3200 vs 3200",'3200vs3200'!D14, "6400 vs 6400",'6400vs6400'!D14, "12800 vs 12800",'12800vs12800'!D14)</f>
@@ -17252,7 +17252,7 @@
       </c>
       <c r="F14" s="9" cm="1">
         <f t="array" ref="F14">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F14, "200 vs 200",'200vs200'!F14, "400 vs 400",'400vs400'!F14, "800 vs 800",'800vs800'!F14, "1600 vs 1600",'1600vs1600'!F14, "3200 vs 3200",'3200vs3200'!F14, "6400 vs 6400",'6400vs6400'!F14, "12800 vs 12800",'12800vs12800'!F14)</f>
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17261,23 +17261,23 @@
       </c>
       <c r="B15" s="9" cm="1">
         <f t="array" ref="B15">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B15, "200 vs 200",'200vs200'!B15, "400 vs 400",'400vs400'!B15, "800 vs 800",'800vs800'!B15, "1600 vs 1600",'1600vs1600'!B15, "3200 vs 3200",'3200vs3200'!B15, "6400 vs 6400",'6400vs6400'!B15, "12800 vs 12800",'12800vs12800'!B15)</f>
-        <v>2.1</v>
+        <v>7.5</v>
       </c>
       <c r="C15" s="9" cm="1">
         <f t="array" ref="C15">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C15, "200 vs 200",'200vs200'!C15, "400 vs 400",'400vs400'!C15, "800 vs 800",'800vs800'!C15, "1600 vs 1600",'1600vs1600'!C15, "3200 vs 3200",'3200vs3200'!C15, "6400 vs 6400",'6400vs6400'!C15, "12800 vs 12800",'12800vs12800'!C15)</f>
-        <v>1.1000000000000001</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D15" s="9" cm="1">
         <f t="array" ref="D15">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D15, "200 vs 200",'200vs200'!D15, "400 vs 400",'400vs400'!D15, "800 vs 800",'800vs800'!D15, "1600 vs 1600",'1600vs1600'!D15, "3200 vs 3200",'3200vs3200'!D15, "6400 vs 6400",'6400vs6400'!D15, "12800 vs 12800",'12800vs12800'!D15)</f>
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="E15" s="9" cm="1">
         <f t="array" ref="E15">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E15, "200 vs 200",'200vs200'!E15, "400 vs 400",'400vs400'!E15, "800 vs 800",'800vs800'!E15, "1600 vs 1600",'1600vs1600'!E15, "3200 vs 3200",'3200vs3200'!E15, "6400 vs 6400",'6400vs6400'!E15, "12800 vs 12800",'12800vs12800'!E15)</f>
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="F15" s="9" cm="1">
         <f t="array" ref="F15">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F15, "200 vs 200",'200vs200'!F15, "400 vs 400",'400vs400'!F15, "800 vs 800",'800vs800'!F15, "1600 vs 1600",'1600vs1600'!F15, "3200 vs 3200",'3200vs3200'!F15, "6400 vs 6400",'6400vs6400'!F15, "12800 vs 12800",'12800vs12800'!F15)</f>
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17286,11 +17286,11 @@
       </c>
       <c r="B16" s="9" cm="1">
         <f t="array" ref="B16">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B16, "200 vs 200",'200vs200'!B16, "400 vs 400",'400vs400'!B16, "800 vs 800",'800vs800'!B16, "1600 vs 1600",'1600vs1600'!B16, "3200 vs 3200",'3200vs3200'!B16, "6400 vs 6400",'6400vs6400'!B16, "12800 vs 12800",'12800vs12800'!B16)</f>
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="C16" s="9" cm="1">
         <f t="array" ref="C16">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C16, "200 vs 200",'200vs200'!C16, "400 vs 400",'400vs400'!C16, "800 vs 800",'800vs800'!C16, "1600 vs 1600",'1600vs1600'!C16, "3200 vs 3200",'3200vs3200'!C16, "6400 vs 6400",'6400vs6400'!C16, "12800 vs 12800",'12800vs12800'!C16)</f>
-        <v>2.2000000000000002</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D16" s="9" cm="1">
         <f t="array" ref="D16">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D16, "200 vs 200",'200vs200'!D16, "400 vs 400",'400vs400'!D16, "800 vs 800",'800vs800'!D16, "1600 vs 1600",'1600vs1600'!D16, "3200 vs 3200",'3200vs3200'!D16, "6400 vs 6400",'6400vs6400'!D16, "12800 vs 12800",'12800vs12800'!D16)</f>
@@ -17298,11 +17298,11 @@
       </c>
       <c r="E16" s="9" cm="1">
         <f t="array" ref="E16">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E16, "200 vs 200",'200vs200'!E16, "400 vs 400",'400vs400'!E16, "800 vs 800",'800vs800'!E16, "1600 vs 1600",'1600vs1600'!E16, "3200 vs 3200",'3200vs3200'!E16, "6400 vs 6400",'6400vs6400'!E16, "12800 vs 12800",'12800vs12800'!E16)</f>
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="F16" s="9" cm="1">
         <f t="array" ref="F16">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F16, "200 vs 200",'200vs200'!F16, "400 vs 400",'400vs400'!F16, "800 vs 800",'800vs800'!F16, "1600 vs 1600",'1600vs1600'!F16, "3200 vs 3200",'3200vs3200'!F16, "6400 vs 6400",'6400vs6400'!F16, "12800 vs 12800",'12800vs12800'!F16)</f>
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -17311,19 +17311,19 @@
       </c>
       <c r="B17" s="10" cm="1">
         <f t="array" ref="B17">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B17, "200 vs 200",'200vs200'!B17, "400 vs 400",'400vs400'!B17, "800 vs 800",'800vs800'!B17, "1600 vs 1600",'1600vs1600'!B17, "3200 vs 3200",'3200vs3200'!B17, "6400 vs 6400",'6400vs6400'!B17, "12800 vs 12800",'12800vs12800'!B17)</f>
-        <v>3.3</v>
+        <v>7.6</v>
       </c>
       <c r="C17" s="10" cm="1">
         <f t="array" ref="C17">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C17, "200 vs 200",'200vs200'!C17, "400 vs 400",'400vs400'!C17, "800 vs 800",'800vs800'!C17, "1600 vs 1600",'1600vs1600'!C17, "3200 vs 3200",'3200vs3200'!C17, "6400 vs 6400",'6400vs6400'!C17, "12800 vs 12800",'12800vs12800'!C17)</f>
-        <v>3.2</v>
+        <v>6</v>
       </c>
       <c r="D17" s="10" cm="1">
         <f t="array" ref="D17">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D17, "200 vs 200",'200vs200'!D17, "400 vs 400",'400vs400'!D17, "800 vs 800",'800vs800'!D17, "1600 vs 1600",'1600vs1600'!D17, "3200 vs 3200",'3200vs3200'!D17, "6400 vs 6400",'6400vs6400'!D17, "12800 vs 12800",'12800vs12800'!D17)</f>
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="E17" s="10" cm="1">
         <f t="array" ref="E17">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E17, "200 vs 200",'200vs200'!E17, "400 vs 400",'400vs400'!E17, "800 vs 800",'800vs800'!E17, "1600 vs 1600",'1600vs1600'!E17, "3200 vs 3200",'3200vs3200'!E17, "6400 vs 6400",'6400vs6400'!E17, "12800 vs 12800",'12800vs12800'!E17)</f>
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="F17" s="10" cm="1">
         <f t="array" ref="F17">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F17, "200 vs 200",'200vs200'!F17, "400 vs 400",'400vs400'!F17, "800 vs 800",'800vs800'!F17, "1600 vs 1600",'1600vs1600'!F17, "3200 vs 3200",'3200vs3200'!F17, "6400 vs 6400",'6400vs6400'!F17, "12800 vs 12800",'12800vs12800'!F17)</f>
@@ -17336,23 +17336,23 @@
       </c>
       <c r="B18" s="9" cm="1">
         <f t="array" ref="B18">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!B18, "200 vs 200",'200vs200'!B18, "400 vs 400",'400vs400'!B18, "800 vs 800",'800vs800'!B18, "1600 vs 1600",'1600vs1600'!B18, "3200 vs 3200",'3200vs3200'!B18, "6400 vs 6400",'6400vs6400'!B18, "12800 vs 12800",'12800vs12800'!B18)</f>
-        <v>2.8000000000000007</v>
+        <v>6.3999999999999986</v>
       </c>
       <c r="C18" s="9" cm="1">
         <f t="array" ref="C18">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!C18, "200 vs 200",'200vs200'!C18, "400 vs 400",'400vs400'!C18, "800 vs 800",'800vs800'!C18, "1600 vs 1600",'1600vs1600'!C18, "3200 vs 3200",'3200vs3200'!C18, "6400 vs 6400",'6400vs6400'!C18, "12800 vs 12800",'12800vs12800'!C18)</f>
-        <v>2.7999999999999989</v>
+        <v>5</v>
       </c>
       <c r="D18" s="9" cm="1">
         <f t="array" ref="D18">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!D18, "200 vs 200",'200vs200'!D18, "400 vs 400",'400vs400'!D18, "800 vs 800",'800vs800'!D18, "1600 vs 1600",'1600vs1600'!D18, "3200 vs 3200",'3200vs3200'!D18, "6400 vs 6400",'6400vs6400'!D18, "12800 vs 12800",'12800vs12800'!D18)</f>
-        <v>2.4000000000000004</v>
+        <v>2.1999999999999993</v>
       </c>
       <c r="E18" s="9" cm="1">
         <f t="array" ref="E18">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!E18, "200 vs 200",'200vs200'!E18, "400 vs 400",'400vs400'!E18, "800 vs 800",'800vs800'!E18, "1600 vs 1600",'1600vs1600'!E18, "3200 vs 3200",'3200vs3200'!E18, "6400 vs 6400",'6400vs6400'!E18, "12800 vs 12800",'12800vs12800'!E18)</f>
-        <v>2.2999999999999998</v>
+        <v>2.0999999999999996</v>
       </c>
       <c r="F18" s="9" cm="1">
         <f t="array" ref="F18">_xlfn.SWITCH($J$1, "100 vs 100",'100vs100'!F18, "200 vs 200",'200vs200'!F18, "400 vs 400",'400vs400'!F18, "800 vs 800",'800vs800'!F18, "1600 vs 1600",'1600vs1600'!F18, "3200 vs 3200",'3200vs3200'!F18, "6400 vs 6400",'6400vs6400'!F18, "12800 vs 12800",'12800vs12800'!F18)</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -17370,8 +17370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4529D9-CDB9-404C-BC65-6587A805F484}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17750,8 +17750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8C534B-81D2-4FA5-A900-ACABFFE2C9A3}">
   <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView topLeftCell="A149" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E186" sqref="E186"/>
+    <sheetView topLeftCell="A143" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M171" sqref="M171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>